<commit_message>
updated mrr sites on shiny website
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20240409.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20240409.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855300B1-5EB3-4ABB-BCE0-1E301F42D359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996A2D5D-1C93-4FD7-A7BF-204CFE4C3C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2405,9 +2405,6 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2415,6 +2412,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2840,7 +2840,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="10" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T38" sqref="T38"/>
+      <selection pane="topRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -2907,16 +2907,16 @@
       <c r="S2" s="140"/>
       <c r="T2" s="140"/>
       <c r="U2" s="140"/>
-      <c r="V2" s="142" t="s">
+      <c r="V2" s="145" t="s">
         <v>422</v>
       </c>
-      <c r="W2" s="142"/>
-      <c r="X2" s="142"/>
-      <c r="Y2" s="142" t="s">
+      <c r="W2" s="145"/>
+      <c r="X2" s="145"/>
+      <c r="Y2" s="145" t="s">
         <v>409</v>
       </c>
-      <c r="Z2" s="142"/>
-      <c r="AA2" s="142"/>
+      <c r="Z2" s="145"/>
+      <c r="AA2" s="145"/>
       <c r="AB2" s="136"/>
     </row>
     <row r="3" spans="2:28" ht="40.799999999999997" x14ac:dyDescent="0.3">
@@ -3040,7 +3040,7 @@
         <v>369</v>
       </c>
       <c r="N4" s="123">
-        <f>VLOOKUP(J4,om_costs,35,FALSE)</f>
+        <f t="shared" ref="N4:N34" si="1">VLOOKUP(J4,om_costs,35,FALSE)</f>
         <v>8006.9800000000005</v>
       </c>
       <c r="O4" s="124">
@@ -3048,14 +3048,14 @@
       </c>
       <c r="P4" s="124"/>
       <c r="Q4" s="123">
-        <f>N4*O4</f>
-        <v>0</v>
-      </c>
-      <c r="R4" s="144" t="s">
+        <f t="shared" ref="Q4:Q34" si="2">N4*O4</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="143" t="s">
         <v>394</v>
       </c>
       <c r="S4" s="128">
-        <f>VLOOKUP(J4,om_costs,27,FALSE)</f>
+        <f t="shared" ref="S4:S34" si="3">VLOOKUP(J4,om_costs,27,FALSE)</f>
         <v>50666</v>
       </c>
       <c r="T4" s="130">
@@ -3074,11 +3074,11 @@
         <v>0</v>
       </c>
       <c r="Z4" s="128">
-        <f t="shared" ref="Z4:AA4" si="1">IF(ISBLANK(W4),0,$S4*$T4)</f>
+        <f t="shared" ref="Z4:AA4" si="4">IF(ISBLANK(W4),0,$S4*$T4)</f>
         <v>40532.800000000003</v>
       </c>
       <c r="AA4" s="128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AB4" s="115" t="s">
@@ -3123,7 +3123,7 @@
         <v>369</v>
       </c>
       <c r="N5" s="123">
-        <f>VLOOKUP(J5,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>8685.7800000000007</v>
       </c>
       <c r="O5" s="124">
@@ -3131,14 +3131,14 @@
       </c>
       <c r="P5" s="124"/>
       <c r="Q5" s="123">
-        <f>N5*O5</f>
-        <v>0</v>
-      </c>
-      <c r="R5" s="144" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="143" t="s">
         <v>395</v>
       </c>
       <c r="S5" s="128">
-        <f>VLOOKUP(J5,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>46054</v>
       </c>
       <c r="T5" s="130">
@@ -3153,15 +3153,15 @@
       <c r="W5" s="130"/>
       <c r="X5" s="130"/>
       <c r="Y5" s="128">
-        <f t="shared" ref="Y5:Y34" si="2">IF(ISBLANK(V5),0,$S5*$T5)</f>
+        <f t="shared" ref="Y5:Y34" si="5">IF(ISBLANK(V5),0,$S5*$T5)</f>
         <v>36843.200000000004</v>
       </c>
       <c r="Z5" s="128">
-        <f t="shared" ref="Z5:Z34" si="3">IF(ISBLANK(W5),0,$S5*$T5)</f>
+        <f t="shared" ref="Z5:Z34" si="6">IF(ISBLANK(W5),0,$S5*$T5)</f>
         <v>0</v>
       </c>
       <c r="AA5" s="128">
-        <f t="shared" ref="AA5:AA34" si="4">IF(ISBLANK(X5),0,$S5*$T5)</f>
+        <f t="shared" ref="AA5:AA34" si="7">IF(ISBLANK(X5),0,$S5*$T5)</f>
         <v>0</v>
       </c>
       <c r="AB5" s="115" t="s">
@@ -3206,7 +3206,7 @@
         <v>369</v>
       </c>
       <c r="N6" s="123">
-        <f>VLOOKUP(J6,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>6277.7</v>
       </c>
       <c r="O6" s="124">
@@ -3214,14 +3214,14 @@
       </c>
       <c r="P6" s="124"/>
       <c r="Q6" s="123">
-        <f>N6*O6</f>
-        <v>0</v>
-      </c>
-      <c r="R6" s="144" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="143" t="s">
         <v>396</v>
       </c>
       <c r="S6" s="128">
-        <f>VLOOKUP(J6,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>44137</v>
       </c>
       <c r="T6" s="130">
@@ -3236,15 +3236,15 @@
       </c>
       <c r="X6" s="130"/>
       <c r="Y6" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z6" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>44137</v>
       </c>
       <c r="AA6" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB6" s="115" t="s">
@@ -3289,7 +3289,7 @@
         <v>369</v>
       </c>
       <c r="N7" s="123">
-        <f>VLOOKUP(J7,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>6956.5</v>
       </c>
       <c r="O7" s="124">
@@ -3297,14 +3297,14 @@
       </c>
       <c r="P7" s="124"/>
       <c r="Q7" s="123">
-        <f>N7*O7</f>
-        <v>0</v>
-      </c>
-      <c r="R7" s="144" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="143" t="s">
         <v>394</v>
       </c>
       <c r="S7" s="128">
-        <f>VLOOKUP(J7,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>39525</v>
       </c>
       <c r="T7" s="130">
@@ -3319,15 +3319,15 @@
         <v>417</v>
       </c>
       <c r="Y7" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z7" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA7" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>31620</v>
       </c>
       <c r="AB7" s="115" t="s">
@@ -3356,7 +3356,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="101">
-        <f t="shared" ref="H8" si="5">G8-F8</f>
+        <f t="shared" ref="H8" si="8">G8-F8</f>
         <v>-5595.2800000000007</v>
       </c>
       <c r="J8" s="106" t="s">
@@ -3372,7 +3372,7 @@
         <v>369</v>
       </c>
       <c r="N8" s="123">
-        <f>VLOOKUP(J8,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>10403.99</v>
       </c>
       <c r="O8" s="124">
@@ -3380,14 +3380,14 @@
       </c>
       <c r="P8" s="124"/>
       <c r="Q8" s="123">
-        <f>N8*O8</f>
-        <v>0</v>
-      </c>
-      <c r="R8" s="144" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="143" t="s">
         <v>427</v>
       </c>
       <c r="S8" s="128">
-        <f>VLOOKUP(J8,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>65578</v>
       </c>
       <c r="T8" s="130">
@@ -3402,15 +3402,15 @@
         <v>417</v>
       </c>
       <c r="Y8" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z8" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA8" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>16394.5</v>
       </c>
       <c r="AB8" s="115" t="s">
@@ -3452,7 +3452,7 @@
         <v>369</v>
       </c>
       <c r="N9" s="123">
-        <f>VLOOKUP(J9,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>10403.99</v>
       </c>
       <c r="O9" s="124">
@@ -3460,14 +3460,14 @@
       </c>
       <c r="P9" s="124"/>
       <c r="Q9" s="123">
-        <f>N9*O9</f>
-        <v>0</v>
-      </c>
-      <c r="R9" s="144" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="143" t="s">
         <v>394</v>
       </c>
       <c r="S9" s="128">
-        <f>VLOOKUP(J9,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>65578</v>
       </c>
       <c r="T9" s="130">
@@ -3482,15 +3482,15 @@
       <c r="W9" s="130"/>
       <c r="X9" s="130"/>
       <c r="Y9" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>52462.400000000001</v>
       </c>
       <c r="Z9" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA9" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB9" s="115" t="s">
@@ -3511,7 +3511,7 @@
         <v>369</v>
       </c>
       <c r="N10" s="123">
-        <f>VLOOKUP(J10,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>9725.19</v>
       </c>
       <c r="O10" s="124">
@@ -3519,14 +3519,14 @@
       </c>
       <c r="P10" s="124"/>
       <c r="Q10" s="123">
-        <f>N10*O10</f>
-        <v>0</v>
-      </c>
-      <c r="R10" s="144" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R10" s="143" t="s">
         <v>394</v>
       </c>
       <c r="S10" s="128">
-        <f>VLOOKUP(J10,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>70190</v>
       </c>
       <c r="T10" s="130">
@@ -3541,15 +3541,15 @@
       </c>
       <c r="X10" s="130"/>
       <c r="Y10" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z10" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>56152</v>
       </c>
       <c r="AA10" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB10" s="115" t="s">
@@ -3570,7 +3570,7 @@
         <v>369</v>
       </c>
       <c r="N11" s="123">
-        <f>VLOOKUP(J11,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>9272.7800000000007</v>
       </c>
       <c r="O11" s="124">
@@ -3578,14 +3578,14 @@
       </c>
       <c r="P11" s="124"/>
       <c r="Q11" s="123">
-        <f>N11*O11</f>
-        <v>0</v>
-      </c>
-      <c r="R11" s="144" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="143" t="s">
         <v>394</v>
       </c>
       <c r="S11" s="128">
-        <f>VLOOKUP(J11,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>51924</v>
       </c>
       <c r="T11" s="130">
@@ -3600,15 +3600,15 @@
       </c>
       <c r="X11" s="130"/>
       <c r="Y11" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z11" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>41539.200000000004</v>
       </c>
       <c r="AA11" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB11" s="115" t="s">
@@ -3631,7 +3631,7 @@
         <v>369</v>
       </c>
       <c r="N12" s="123">
-        <f>VLOOKUP(J12,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>4852.5</v>
       </c>
       <c r="O12" s="124">
@@ -3641,14 +3641,14 @@
         <v>411</v>
       </c>
       <c r="Q12" s="123">
-        <f>N12*O12</f>
-        <v>0</v>
-      </c>
-      <c r="R12" s="144" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="143" t="s">
         <v>394</v>
       </c>
       <c r="S12" s="128">
-        <f>VLOOKUP(J12,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>36525</v>
       </c>
       <c r="T12" s="130">
@@ -3663,15 +3663,15 @@
         <v>417</v>
       </c>
       <c r="Y12" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z12" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA12" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>29220</v>
       </c>
       <c r="AB12" s="115" t="s">
@@ -3694,7 +3694,7 @@
         <v>369</v>
       </c>
       <c r="N13" s="123">
-        <f>VLOOKUP(J13,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>9386.619999999999</v>
       </c>
       <c r="O13" s="124">
@@ -3704,14 +3704,14 @@
         <v>411</v>
       </c>
       <c r="Q13" s="123">
-        <f>N13*O13</f>
-        <v>0</v>
-      </c>
-      <c r="R13" s="144" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S13" s="128">
-        <f>VLOOKUP(J13,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>61778</v>
       </c>
       <c r="T13" s="130"/>
@@ -3722,15 +3722,15 @@
       <c r="W13" s="130"/>
       <c r="X13" s="130"/>
       <c r="Y13" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z13" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA13" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB13" s="115" t="s">
@@ -3753,7 +3753,7 @@
         <v>369</v>
       </c>
       <c r="N14" s="123">
-        <f>VLOOKUP(J14,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>12531.68</v>
       </c>
       <c r="O14" s="124">
@@ -3761,14 +3761,14 @@
       </c>
       <c r="P14" s="124"/>
       <c r="Q14" s="123">
-        <f>N14*O14</f>
+        <f t="shared" si="2"/>
         <v>12531.68</v>
       </c>
-      <c r="R14" s="144" t="s">
+      <c r="R14" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S14" s="128">
-        <f>VLOOKUP(J14,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>119096</v>
       </c>
       <c r="T14" s="130"/>
@@ -3779,15 +3779,15 @@
       <c r="W14" s="130"/>
       <c r="X14" s="130"/>
       <c r="Y14" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z14" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA14" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB14" s="115" t="s">
@@ -3810,7 +3810,7 @@
         <v>369</v>
       </c>
       <c r="N15" s="123">
-        <f>VLOOKUP(J15,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>12130.16</v>
       </c>
       <c r="O15" s="124">
@@ -3818,14 +3818,14 @@
       </c>
       <c r="P15" s="124"/>
       <c r="Q15" s="123">
-        <f>N15*O15</f>
+        <f t="shared" si="2"/>
         <v>12130.16</v>
       </c>
-      <c r="R15" s="144" t="s">
+      <c r="R15" s="143" t="s">
         <v>424</v>
       </c>
       <c r="S15" s="128">
-        <f>VLOOKUP(J15,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>114077</v>
       </c>
       <c r="T15" s="130">
@@ -3840,15 +3840,15 @@
         <v>417</v>
       </c>
       <c r="Y15" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z15" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA15" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>114077</v>
       </c>
       <c r="AB15" s="115" t="s">
@@ -3871,7 +3871,7 @@
         <v>369</v>
       </c>
       <c r="N16" s="123">
-        <f>VLOOKUP(J16,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>9058.4000000000015</v>
       </c>
       <c r="O16" s="124">
@@ -3881,14 +3881,14 @@
         <v>434</v>
       </c>
       <c r="Q16" s="123">
-        <f>N16*O16</f>
-        <v>0</v>
-      </c>
-      <c r="R16" s="144" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S16" s="128">
-        <f>VLOOKUP(J16,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>77180</v>
       </c>
       <c r="T16" s="130"/>
@@ -3899,15 +3899,15 @@
       <c r="W16" s="130"/>
       <c r="X16" s="130"/>
       <c r="Y16" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z16" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA16" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB16" s="115" t="s">
@@ -3930,7 +3930,7 @@
         <v>369</v>
       </c>
       <c r="N17" s="123">
-        <f>VLOOKUP(J17,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>5268.24</v>
       </c>
       <c r="O17" s="124">
@@ -3938,14 +3938,14 @@
       </c>
       <c r="P17" s="124"/>
       <c r="Q17" s="123">
-        <f>N17*O17</f>
+        <f t="shared" si="2"/>
         <v>5268.24</v>
       </c>
-      <c r="R17" s="144" t="s">
+      <c r="R17" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S17" s="128">
-        <f>VLOOKUP(J17,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>42553</v>
       </c>
       <c r="T17" s="130"/>
@@ -3956,15 +3956,15 @@
       <c r="W17" s="130"/>
       <c r="X17" s="130"/>
       <c r="Y17" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z17" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA17" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB17" s="115" t="s">
@@ -3987,7 +3987,7 @@
         <v>369</v>
       </c>
       <c r="N18" s="123">
-        <f>VLOOKUP(J18,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>8583.58</v>
       </c>
       <c r="O18" s="124">
@@ -3995,14 +3995,14 @@
       </c>
       <c r="P18" s="124"/>
       <c r="Q18" s="123">
-        <f>N18*O18</f>
+        <f t="shared" si="2"/>
         <v>8583.58</v>
       </c>
-      <c r="R18" s="144" t="s">
+      <c r="R18" s="143" t="s">
         <v>397</v>
       </c>
       <c r="S18" s="128">
-        <f>VLOOKUP(J18,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>51740</v>
       </c>
       <c r="T18" s="130">
@@ -4017,15 +4017,15 @@
       <c r="W18" s="130"/>
       <c r="X18" s="130"/>
       <c r="Y18" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1552.2</v>
       </c>
       <c r="Z18" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA18" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB18" s="115" t="s">
@@ -4048,7 +4048,7 @@
         <v>369</v>
       </c>
       <c r="N19" s="123">
-        <f>VLOOKUP(J19,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>11224.67</v>
       </c>
       <c r="O19" s="124">
@@ -4056,14 +4056,14 @@
       </c>
       <c r="P19" s="124"/>
       <c r="Q19" s="123">
-        <f>N19*O19</f>
+        <f t="shared" si="2"/>
         <v>11224.67</v>
       </c>
-      <c r="R19" s="144" t="s">
+      <c r="R19" s="143" t="s">
         <v>397</v>
       </c>
       <c r="S19" s="128">
-        <f>VLOOKUP(J19,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>83249</v>
       </c>
       <c r="T19" s="130">
@@ -4078,15 +4078,15 @@
       <c r="W19" s="130"/>
       <c r="X19" s="130"/>
       <c r="Y19" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2497.4699999999998</v>
       </c>
       <c r="Z19" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA19" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB19" s="115" t="s">
@@ -4109,7 +4109,7 @@
         <v>369</v>
       </c>
       <c r="N20" s="123">
-        <f>VLOOKUP(J20,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>6910.4</v>
       </c>
       <c r="O20" s="124">
@@ -4117,14 +4117,14 @@
       </c>
       <c r="P20" s="124"/>
       <c r="Q20" s="123">
-        <f>N20*O20</f>
+        <f t="shared" si="2"/>
         <v>6910.4</v>
       </c>
-      <c r="R20" s="144" t="s">
+      <c r="R20" s="143" t="s">
         <v>426</v>
       </c>
       <c r="S20" s="128">
-        <f>VLOOKUP(J20,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>48830</v>
       </c>
       <c r="T20" s="130">
@@ -4139,15 +4139,15 @@
       </c>
       <c r="X20" s="130"/>
       <c r="Y20" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z20" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9766</v>
       </c>
       <c r="AA20" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB20" s="115" t="s">
@@ -4170,7 +4170,7 @@
         <v>369</v>
       </c>
       <c r="N21" s="123">
-        <f>VLOOKUP(J21,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>5595.2800000000007</v>
       </c>
       <c r="O21" s="124">
@@ -4178,14 +4178,14 @@
       </c>
       <c r="P21" s="124"/>
       <c r="Q21" s="123">
-        <f>N21*O21</f>
+        <f t="shared" si="2"/>
         <v>5595.2800000000007</v>
       </c>
-      <c r="R21" s="144" t="s">
+      <c r="R21" s="143" t="s">
         <v>397</v>
       </c>
       <c r="S21" s="128">
-        <f>VLOOKUP(J21,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>51191</v>
       </c>
       <c r="T21" s="130">
@@ -4200,15 +4200,15 @@
       </c>
       <c r="X21" s="130"/>
       <c r="Y21" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z21" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2047.64</v>
       </c>
       <c r="AA21" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB21" s="115" t="s">
@@ -4231,7 +4231,7 @@
         <v>363</v>
       </c>
       <c r="N22" s="123">
-        <f>VLOOKUP(J22,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>6277.7</v>
       </c>
       <c r="O22" s="124">
@@ -4239,14 +4239,14 @@
       </c>
       <c r="P22" s="124"/>
       <c r="Q22" s="123">
-        <f>N22*O22</f>
+        <f t="shared" si="2"/>
         <v>-6277.7</v>
       </c>
-      <c r="R22" s="144" t="s">
+      <c r="R22" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S22" s="128">
-        <f>VLOOKUP(J22,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>44137</v>
       </c>
       <c r="T22" s="130">
@@ -4261,15 +4261,15 @@
         <v>417</v>
       </c>
       <c r="Y22" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z22" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA22" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6620.55</v>
       </c>
       <c r="AB22" s="115" t="s">
@@ -4290,7 +4290,7 @@
         <v>363</v>
       </c>
       <c r="N23" s="123">
-        <f>VLOOKUP(J23,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>3984.32</v>
       </c>
       <c r="O23" s="124">
@@ -4298,14 +4298,14 @@
       </c>
       <c r="P23" s="124"/>
       <c r="Q23" s="123">
-        <f>N23*O23</f>
+        <f t="shared" si="2"/>
         <v>-3984.32</v>
       </c>
-      <c r="R23" s="144" t="s">
+      <c r="R23" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S23" s="128">
-        <f>VLOOKUP(J23,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>28004</v>
       </c>
       <c r="T23" s="130">
@@ -4320,15 +4320,15 @@
         <v>417</v>
       </c>
       <c r="Y23" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z23" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA23" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4200.5999999999995</v>
       </c>
       <c r="AB23" s="115" t="s">
@@ -4349,7 +4349,7 @@
         <v>392</v>
       </c>
       <c r="N24" s="123">
-        <f>VLOOKUP(J24,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>4289.12</v>
       </c>
       <c r="O24" s="124">
@@ -4357,14 +4357,14 @@
       </c>
       <c r="P24" s="124"/>
       <c r="Q24" s="123">
-        <f>N24*O24</f>
+        <f t="shared" si="2"/>
         <v>-4289.12</v>
       </c>
-      <c r="R24" s="144" t="s">
+      <c r="R24" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S24" s="128">
-        <f>VLOOKUP(J24,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>29539</v>
       </c>
       <c r="T24" s="130">
@@ -4379,15 +4379,15 @@
         <v>417</v>
       </c>
       <c r="Y24" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z24" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA24" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4430.8499999999995</v>
       </c>
       <c r="AB24" s="115" t="s">
@@ -4408,7 +4408,7 @@
         <v>363</v>
       </c>
       <c r="N25" s="123">
-        <f>VLOOKUP(J25,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>3509.2</v>
       </c>
       <c r="O25" s="124">
@@ -4416,14 +4416,14 @@
       </c>
       <c r="P25" s="124"/>
       <c r="Q25" s="123">
-        <f>N25*O25</f>
+        <f t="shared" si="2"/>
         <v>-3509.2</v>
       </c>
-      <c r="R25" s="144" t="s">
+      <c r="R25" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S25" s="128">
-        <f>VLOOKUP(J25,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>20565</v>
       </c>
       <c r="T25" s="130">
@@ -4438,15 +4438,15 @@
         <v>417</v>
       </c>
       <c r="Y25" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z25" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA25" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3084.75</v>
       </c>
       <c r="AB25" s="115" t="s">
@@ -4467,7 +4467,7 @@
         <v>363</v>
       </c>
       <c r="N26" s="123">
-        <f>VLOOKUP(J26,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>3442.4</v>
       </c>
       <c r="O26" s="124">
@@ -4475,14 +4475,14 @@
       </c>
       <c r="P26" s="124"/>
       <c r="Q26" s="123">
-        <f>N26*O26</f>
+        <f t="shared" si="2"/>
         <v>-3442.4</v>
       </c>
-      <c r="R26" s="144" t="s">
+      <c r="R26" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S26" s="128">
-        <f>VLOOKUP(J26,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>19730</v>
       </c>
       <c r="T26" s="130">
@@ -4497,15 +4497,15 @@
         <v>417</v>
       </c>
       <c r="Y26" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z26" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA26" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2959.5</v>
       </c>
       <c r="AB26" s="115" t="s">
@@ -4526,7 +4526,7 @@
         <v>7</v>
       </c>
       <c r="N27" s="123">
-        <f>VLOOKUP(J27,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>11204.91</v>
       </c>
       <c r="O27" s="124">
@@ -4534,14 +4534,14 @@
       </c>
       <c r="P27" s="124"/>
       <c r="Q27" s="123">
-        <f>N27*O27</f>
+        <f t="shared" si="2"/>
         <v>-11204.91</v>
       </c>
-      <c r="R27" s="144" t="s">
+      <c r="R27" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S27" s="128">
-        <f>VLOOKUP(J27,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>94259</v>
       </c>
       <c r="T27" s="130"/>
@@ -4552,15 +4552,15 @@
       <c r="W27" s="130"/>
       <c r="X27" s="130"/>
       <c r="Y27" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z27" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA27" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB27" s="115" t="s">
@@ -4581,7 +4581,7 @@
         <v>363</v>
       </c>
       <c r="N28" s="123">
-        <f>VLOOKUP(J28,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>8685.7800000000007</v>
       </c>
       <c r="O28" s="124">
@@ -4589,14 +4589,14 @@
       </c>
       <c r="P28" s="124"/>
       <c r="Q28" s="123">
-        <f>N28*O28</f>
+        <f t="shared" si="2"/>
         <v>-8685.7800000000007</v>
       </c>
-      <c r="R28" s="144" t="s">
+      <c r="R28" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S28" s="128">
-        <f>VLOOKUP(J28,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>46054</v>
       </c>
       <c r="T28" s="130">
@@ -4611,15 +4611,15 @@
       <c r="W28" s="130"/>
       <c r="X28" s="130"/>
       <c r="Y28" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6908.0999999999995</v>
       </c>
       <c r="Z28" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA28" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB28" s="115" t="s">
@@ -4640,7 +4640,7 @@
         <v>363</v>
       </c>
       <c r="N29" s="123">
-        <f>VLOOKUP(J29,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>7348.7800000000007</v>
       </c>
       <c r="O29" s="124">
@@ -4648,14 +4648,14 @@
       </c>
       <c r="P29" s="124"/>
       <c r="Q29" s="123">
-        <f>N29*O29</f>
+        <f t="shared" si="2"/>
         <v>-7348.7800000000007</v>
       </c>
-      <c r="R29" s="144" t="s">
+      <c r="R29" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S29" s="128">
-        <f>VLOOKUP(J29,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>32684</v>
       </c>
       <c r="T29" s="130">
@@ -4670,15 +4670,15 @@
       <c r="W29" s="130"/>
       <c r="X29" s="130"/>
       <c r="Y29" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4902.5999999999995</v>
       </c>
       <c r="Z29" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA29" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB29" s="115" t="s">
@@ -4699,7 +4699,7 @@
         <v>363</v>
       </c>
       <c r="N30" s="123">
-        <f>VLOOKUP(J30,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>10697.49</v>
       </c>
       <c r="O30" s="124">
@@ -4707,14 +4707,14 @@
       </c>
       <c r="P30" s="124"/>
       <c r="Q30" s="123">
-        <f>N30*O30</f>
+        <f t="shared" si="2"/>
         <v>-10697.49</v>
       </c>
-      <c r="R30" s="144" t="s">
+      <c r="R30" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S30" s="128">
-        <f>VLOOKUP(J30,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>68513</v>
       </c>
       <c r="T30" s="130">
@@ -4729,15 +4729,15 @@
       </c>
       <c r="X30" s="130"/>
       <c r="Y30" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z30" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>10276.949999999999</v>
       </c>
       <c r="AA30" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB30" s="115" t="s">
@@ -4758,7 +4758,7 @@
         <v>369</v>
       </c>
       <c r="N31" s="123">
-        <f>VLOOKUP(J31,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>13627.71</v>
       </c>
       <c r="O31" s="124">
@@ -4768,14 +4768,14 @@
         <v>413</v>
       </c>
       <c r="Q31" s="123">
-        <f>N31*O31</f>
-        <v>0</v>
-      </c>
-      <c r="R31" s="144" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R31" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S31" s="128">
-        <f>VLOOKUP(J31,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>95287</v>
       </c>
       <c r="T31" s="130"/>
@@ -4786,15 +4786,15 @@
       <c r="W31" s="130"/>
       <c r="X31" s="130"/>
       <c r="Y31" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z31" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA31" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB31" s="115" t="s">
@@ -4815,7 +4815,7 @@
         <v>369</v>
       </c>
       <c r="N32" s="123">
-        <f>VLOOKUP(J32,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>13627.71</v>
       </c>
       <c r="O32" s="124">
@@ -4825,14 +4825,14 @@
         <v>413</v>
       </c>
       <c r="Q32" s="123">
-        <f>N32*O32</f>
-        <v>0</v>
-      </c>
-      <c r="R32" s="144" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R32" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S32" s="128">
-        <f>VLOOKUP(J32,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>95287</v>
       </c>
       <c r="T32" s="130"/>
@@ -4843,15 +4843,15 @@
       <c r="W32" s="130"/>
       <c r="X32" s="130"/>
       <c r="Y32" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z32" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA32" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB32" s="115" t="s">
@@ -4872,7 +4872,7 @@
         <v>369</v>
       </c>
       <c r="N33" s="123">
-        <f>VLOOKUP(J33,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>10803.39</v>
       </c>
       <c r="O33" s="124">
@@ -4882,14 +4882,14 @@
         <v>412</v>
       </c>
       <c r="Q33" s="123">
-        <f>N33*O33</f>
-        <v>0</v>
-      </c>
-      <c r="R33" s="144" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R33" s="143" t="s">
         <v>377</v>
       </c>
       <c r="S33" s="128">
-        <f>VLOOKUP(J33,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>89240</v>
       </c>
       <c r="T33" s="130"/>
@@ -4900,15 +4900,15 @@
       <c r="W33" s="130"/>
       <c r="X33" s="130"/>
       <c r="Y33" s="128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z33" s="128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA33" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB33" s="115" t="s">
@@ -4929,7 +4929,7 @@
         <v>369</v>
       </c>
       <c r="N34" s="125">
-        <f>VLOOKUP(J34,om_costs,35,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>6874.32</v>
       </c>
       <c r="O34" s="126">
@@ -4939,14 +4939,14 @@
         <v>412</v>
       </c>
       <c r="Q34" s="125">
-        <f>N34*O34</f>
-        <v>0</v>
-      </c>
-      <c r="R34" s="145" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R34" s="144" t="s">
         <v>377</v>
       </c>
       <c r="S34" s="129">
-        <f>VLOOKUP(J34,om_costs,27,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>62629</v>
       </c>
       <c r="T34" s="131"/>
@@ -4957,15 +4957,15 @@
       <c r="W34" s="131"/>
       <c r="X34" s="131"/>
       <c r="Y34" s="129">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z34" s="129">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA34" s="129">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB34" s="117" t="s">
@@ -4982,7 +4982,7 @@
         <v>2804.3100000000013</v>
       </c>
       <c r="R35" s="113"/>
-      <c r="X35" s="143" t="s">
+      <c r="X35" s="142" t="s">
         <v>423</v>
       </c>
       <c r="Y35" s="132">
@@ -4990,16 +4990,16 @@
         <v>105165.97000000002</v>
       </c>
       <c r="Z35" s="132">
-        <f t="shared" ref="Z35:AA35" si="6">SUM(Z4:Z34)</f>
+        <f t="shared" ref="Z35:AA35" si="9">SUM(Z4:Z34)</f>
         <v>204451.59000000003</v>
       </c>
       <c r="AA35" s="132">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>212607.75</v>
       </c>
     </row>
     <row r="36" spans="10:28" x14ac:dyDescent="0.3">
-      <c r="X36" s="143" t="s">
+      <c r="X36" s="142" t="s">
         <v>425</v>
       </c>
       <c r="Y36" s="132">

</xml_diff>

<commit_message>
notes about BRC operations for SY23 & 24 chnk
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20240409.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20240409.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996A2D5D-1C93-4FD7-A7BF-204CFE4C3C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB182AD-413B-4426-BBC4-DCC02287E343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Planning" sheetId="4" r:id="rId1"/>
@@ -2838,9 +2838,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC6A41C-4EE9-4E25-91C6-882C326C1FB9}">
   <dimension ref="B2:AB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="10" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G12" sqref="G12"/>
+      <selection pane="topRight" activeCell="J33" sqref="J33:N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -5030,7 +5030,7 @@
   <dimension ref="A1:AI62"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="Z7" activeCellId="2" sqref="V7 X7 Z7"/>

</xml_diff>

<commit_message>
updated info in iptds o&m costs
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20240409.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20240409.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD37A85-D1DC-4F92-9DE7-3FC5DE52BEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4132169B-D6D4-4AE5-8DDC-F8DB022A1B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,6 +57,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Mike Ackerman</author>
+    <author>tc={010A182B-A551-4254-B23A-44D962FA2B27}</author>
   </authors>
   <commentList>
     <comment ref="P3" authorId="0" shapeId="0" xr:uid="{F84C0372-05FE-4CA8-8C1B-39CB2832F8A8}">
@@ -85,6 +86,14 @@
 * Decommission: -1
 I.e., Continue funding doesn't affect annual O&amp;M costs; new sites will increase costs, and decommissioned sites will lower costs.</t>
         </r>
+      </text>
+    </comment>
+    <comment ref="Q35" authorId="1" shapeId="0" xr:uid="{010A182B-A551-4254-B23A-44D962FA2B27}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Difference btw this amount &amp; cell H3 is equal to O&amp;M costs for YFK, PCA.</t>
       </text>
     </comment>
   </commentList>
@@ -452,7 +461,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2130" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2133" uniqueCount="444">
   <si>
     <t>WDFW</t>
   </si>
@@ -1573,18 +1582,9 @@
     <t>Totals:</t>
   </si>
   <si>
-    <t>USI, CAC, BTL, LLS, BHC, SFG, BSC, COC, IR2</t>
-  </si>
-  <si>
     <t>Change in Sites</t>
   </si>
   <si>
-    <t>SFG, BSC</t>
-  </si>
-  <si>
-    <t>SW1, SW2, SC4, LAP, WR2, MR1</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -1618,9 +1618,6 @@
     <t>NOAA, PSMFC</t>
   </si>
   <si>
-    <t>PCA, YFK, SW1, SW2, SC4, LAP, WR2, MR1, WEN, USC, USP, CHA, LSR, ACM</t>
-  </si>
-  <si>
     <t>Transfer In</t>
   </si>
   <si>
@@ -1781,6 +1778,59 @@
   </si>
   <si>
     <t>Ideally, site evaluations would occur in 2025 with installation in 2026 or 2027.</t>
+  </si>
+  <si>
+    <t>PCA, YFK, SW1, SW2, LAP, WR2, MR1, WEN, ACM</t>
+  </si>
+  <si>
+    <t>SW1, SW2, LAP, WR2, MR1</t>
+  </si>
+  <si>
+    <t>NPT Research</t>
+  </si>
+  <si>
+    <t>NPT Watershed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">USI, CAC, BTL, LLS, BHC, SFG, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>BSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>COC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, IR2</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1793,7 +1843,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1863,6 +1913,12 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2066,7 +2122,7 @@
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2417,6 +2473,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2714,6 +2773,14 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="Q35" dT="2025-07-24T14:41:36.33" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{010A182B-A551-4254-B23A-44D962FA2B27}">
+    <text>Difference btw this amount &amp; cell H3 is equal to O&amp;M costs for YFK, PCA.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="R27" dT="2024-08-14T18:59:14.38" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{73EDD025-783F-4768-B6C6-6E6621A2EF01}">
     <text>Uncertain</text>
   </threadedComment>
@@ -2840,7 +2907,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="10" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J33" sqref="J33:N34"/>
+      <selection pane="topRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -2850,9 +2917,8 @@
     <col min="3" max="3" width="16.33203125" style="106" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="106" customWidth="1"/>
     <col min="5" max="5" width="8.77734375" style="93" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" style="96" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="96" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="96" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" style="96" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="96" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="1.77734375" style="96" customWidth="1"/>
     <col min="10" max="10" width="11.88671875" style="96" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="33.77734375" style="96" bestFit="1" customWidth="1"/>
@@ -2861,14 +2927,15 @@
     <col min="14" max="14" width="9.88671875" style="96" customWidth="1"/>
     <col min="15" max="15" width="5.5546875" style="96" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.77734375" style="96" customWidth="1"/>
-    <col min="17" max="17" width="11" style="96" customWidth="1"/>
+    <col min="17" max="17" width="12.21875" style="96" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22.88671875" style="114" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.6640625" style="96" customWidth="1"/>
     <col min="20" max="20" width="5.5546875" style="96" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6.21875" style="96" customWidth="1"/>
     <col min="22" max="22" width="4.33203125" style="96" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="8.21875" style="96" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="10.44140625" style="96" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.88671875" style="96" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="13.21875" style="96" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="58.88671875" style="96" customWidth="1"/>
     <col min="29" max="16384" width="8.77734375" style="96"/>
   </cols>
@@ -2878,22 +2945,22 @@
         <v>371</v>
       </c>
       <c r="C2" s="119" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D2" s="119" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="E2" s="121" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F2" s="118" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G2" s="118" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="H2" s="118" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="J2" s="136"/>
       <c r="K2" s="136"/>
@@ -2908,29 +2975,29 @@
       <c r="T2" s="140"/>
       <c r="U2" s="140"/>
       <c r="V2" s="145" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="W2" s="145"/>
       <c r="X2" s="145"/>
       <c r="Y2" s="145" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="Z2" s="145"/>
       <c r="AA2" s="145"/>
       <c r="AB2" s="136"/>
     </row>
-    <row r="3" spans="2:28" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:28" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
         <v>369</v>
       </c>
       <c r="C3" s="92" t="s">
-        <v>388</v>
+        <v>439</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>373</v>
+        <v>443</v>
       </c>
       <c r="E3" s="93">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F3" s="94">
         <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B3,'O&amp;M Costs'!$AI$2:$AI$50)</f>
@@ -2938,11 +3005,11 @@
       </c>
       <c r="G3" s="94">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B3,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>351238.12000000005</v>
+        <v>297246.59000000003</v>
       </c>
       <c r="H3" s="95">
         <f>G3-F3</f>
-        <v>71034.960000000021</v>
+        <v>17043.429999999993</v>
       </c>
       <c r="J3" s="89" t="s">
         <v>103</v>
@@ -2954,78 +3021,78 @@
         <v>367</v>
       </c>
       <c r="M3" s="89" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="N3" s="137" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="O3" s="137" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="P3" s="137" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="Q3" s="137" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="R3" s="138" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="S3" s="138" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="T3" s="138" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="U3" s="138" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="V3" s="138">
         <v>2025</v>
       </c>
       <c r="W3" s="138" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="X3" s="138" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="Y3" s="138">
         <v>2025</v>
       </c>
       <c r="Z3" s="138" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="AA3" s="138" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="AB3" s="88" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
-    <row r="4" spans="2:28" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:28" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="91" t="s">
-        <v>7</v>
+        <v>441</v>
       </c>
       <c r="C4" s="92" t="s">
-        <v>375</v>
+        <v>47</v>
       </c>
       <c r="D4" s="92" t="s">
-        <v>376</v>
+        <v>440</v>
       </c>
       <c r="E4" s="93">
         <v>-4</v>
       </c>
       <c r="F4" s="94">
         <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B4,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>66249.05</v>
+        <v>49738.33</v>
       </c>
       <c r="G4" s="94">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B4,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>27343.010000000002</v>
+        <v>11204.91</v>
       </c>
       <c r="H4" s="95">
-        <f t="shared" ref="H4:H7" si="0">G4-F4</f>
-        <v>-38906.04</v>
+        <f t="shared" ref="H4:H8" si="0">G4-F4</f>
+        <v>-38533.42</v>
       </c>
       <c r="J4" s="106" t="s">
         <v>74</v>
@@ -3052,7 +3119,7 @@
         <v>0</v>
       </c>
       <c r="R4" s="143" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="S4" s="128">
         <f t="shared" ref="S4:S34" si="3">VLOOKUP(J4,om_costs,27,FALSE)</f>
@@ -3062,11 +3129,11 @@
         <v>0.8</v>
       </c>
       <c r="U4" s="130" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="V4" s="130"/>
       <c r="W4" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="X4" s="130"/>
       <c r="Y4" s="128">
@@ -3082,33 +3149,33 @@
         <v>0</v>
       </c>
       <c r="AB4" s="115" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="91" t="s">
-        <v>36</v>
+        <v>442</v>
       </c>
       <c r="C5" s="92" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D5" s="92" t="s">
-        <v>34</v>
+        <v>374</v>
       </c>
       <c r="E5" s="93">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="94">
         <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B5,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>6910.4</v>
+        <v>16510.72</v>
       </c>
       <c r="G5" s="94">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B5,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>0</v>
+        <v>16510.72</v>
       </c>
       <c r="H5" s="95">
         <f t="shared" si="0"/>
-        <v>-6910.4</v>
+        <v>0</v>
       </c>
       <c r="J5" s="106" t="s">
         <v>237</v>
@@ -3135,7 +3202,7 @@
         <v>0</v>
       </c>
       <c r="R5" s="143" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="S5" s="128">
         <f t="shared" si="3"/>
@@ -3145,10 +3212,10 @@
         <v>0.8</v>
       </c>
       <c r="U5" s="130" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="V5" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="W5" s="130"/>
       <c r="X5" s="130"/>
@@ -3165,25 +3232,25 @@
         <v>0</v>
       </c>
       <c r="AB5" s="115" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
-    <row r="6" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="91" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C6" s="92" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D6" s="92" t="s">
-        <v>378</v>
+        <v>34</v>
       </c>
       <c r="E6" s="93">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="F6" s="94">
         <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B6,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>14239.119999999999</v>
+        <v>6910.4</v>
       </c>
       <c r="G6" s="94">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B6,'O&amp;M Costs'!$AI$2:$AI$50)</f>
@@ -3191,7 +3258,7 @@
       </c>
       <c r="H6" s="95">
         <f t="shared" si="0"/>
-        <v>-14239.119999999999</v>
+        <v>-6910.4</v>
       </c>
       <c r="J6" s="106" t="s">
         <v>15</v>
@@ -3218,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="143" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="S6" s="128">
         <f t="shared" si="3"/>
@@ -3228,11 +3295,11 @@
         <v>1</v>
       </c>
       <c r="U6" s="130" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="V6" s="130"/>
       <c r="W6" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="X6" s="130"/>
       <c r="Y6" s="128">
@@ -3248,33 +3315,33 @@
         <v>0</v>
       </c>
       <c r="AB6" s="115" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B7" s="107" t="s">
-        <v>370</v>
-      </c>
-      <c r="C7" s="108" t="s">
-        <v>379</v>
-      </c>
-      <c r="D7" s="108" t="s">
-        <v>377</v>
-      </c>
-      <c r="E7" s="109">
-        <v>4</v>
-      </c>
-      <c r="F7" s="110">
+    <row r="7" spans="2:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="91" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="92" t="s">
+        <v>374</v>
+      </c>
+      <c r="D7" s="92" t="s">
+        <v>375</v>
+      </c>
+      <c r="E7" s="93">
+        <v>-2</v>
+      </c>
+      <c r="F7" s="94">
         <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B7,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="110">
+        <v>14239.119999999999</v>
+      </c>
+      <c r="G7" s="94">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B7,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>15225.039999999999</v>
-      </c>
-      <c r="H7" s="111">
+        <v>0</v>
+      </c>
+      <c r="H7" s="95">
         <f t="shared" si="0"/>
-        <v>15225.039999999999</v>
+        <v>-14239.119999999999</v>
       </c>
       <c r="J7" s="106" t="s">
         <v>9</v>
@@ -3301,7 +3368,7 @@
         <v>0</v>
       </c>
       <c r="R7" s="143" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="S7" s="128">
         <f t="shared" si="3"/>
@@ -3311,12 +3378,12 @@
         <v>0.8</v>
       </c>
       <c r="U7" s="130" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="V7" s="130"/>
       <c r="W7" s="130"/>
       <c r="X7" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="Y7" s="128">
         <f t="shared" si="5"/>
@@ -3331,33 +3398,33 @@
         <v>31620</v>
       </c>
       <c r="AB7" s="115" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8" spans="2:28" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="98" t="s">
-        <v>377</v>
-      </c>
-      <c r="D8" s="98" t="s">
-        <v>383</v>
-      </c>
-      <c r="E8" s="99">
-        <v>-1</v>
-      </c>
-      <c r="F8" s="100">
+      <c r="B8" s="107" t="s">
+        <v>370</v>
+      </c>
+      <c r="C8" s="108" t="s">
+        <v>376</v>
+      </c>
+      <c r="D8" s="108" t="s">
+        <v>374</v>
+      </c>
+      <c r="E8" s="109">
+        <v>4</v>
+      </c>
+      <c r="F8" s="110">
         <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B8,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>5595.2800000000007</v>
-      </c>
-      <c r="G8" s="100">
+        <v>0</v>
+      </c>
+      <c r="G8" s="110">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B8,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="101">
-        <f t="shared" ref="H8" si="8">G8-F8</f>
-        <v>-5595.2800000000007</v>
+        <v>15225.039999999999</v>
+      </c>
+      <c r="H8" s="111">
+        <f t="shared" si="0"/>
+        <v>15225.039999999999</v>
       </c>
       <c r="J8" s="106" t="s">
         <v>11</v>
@@ -3384,7 +3451,7 @@
         <v>0</v>
       </c>
       <c r="R8" s="143" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="S8" s="128">
         <f t="shared" si="3"/>
@@ -3394,12 +3461,12 @@
         <v>0.25</v>
       </c>
       <c r="U8" s="130" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="V8" s="130"/>
       <c r="W8" s="130"/>
       <c r="X8" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="Y8" s="128">
         <f t="shared" si="5"/>
@@ -3414,30 +3481,33 @@
         <v>16394.5</v>
       </c>
       <c r="AB8" s="115" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="9" spans="2:28" s="105" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="102" t="s">
-        <v>372</v>
-      </c>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="103">
-        <f>SUM(E3:E8)</f>
-        <v>1</v>
-      </c>
-      <c r="F9" s="104">
-        <f>SUM(F3:F8)</f>
-        <v>373197.01000000007</v>
-      </c>
-      <c r="G9" s="104">
-        <f>SUM(G3:G8)</f>
-        <v>393806.17000000004</v>
-      </c>
-      <c r="H9" s="104">
-        <f>SUM(H3:H8)</f>
-        <v>20609.160000000018</v>
+      <c r="B9" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="98" t="s">
+        <v>374</v>
+      </c>
+      <c r="D9" s="98" t="s">
+        <v>380</v>
+      </c>
+      <c r="E9" s="99">
+        <v>-1</v>
+      </c>
+      <c r="F9" s="100">
+        <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B9,'O&amp;M Costs'!$AI$2:$AI$50)</f>
+        <v>5595.2800000000007</v>
+      </c>
+      <c r="G9" s="100">
+        <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B9,'O&amp;M Costs'!$AI$2:$AI$50)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="101">
+        <f t="shared" ref="H9" si="8">G9-F9</f>
+        <v>-5595.2800000000007</v>
       </c>
       <c r="J9" s="106" t="s">
         <v>86</v>
@@ -3464,7 +3534,7 @@
         <v>0</v>
       </c>
       <c r="R9" s="143" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="S9" s="128">
         <f t="shared" si="3"/>
@@ -3474,10 +3544,10 @@
         <v>0.8</v>
       </c>
       <c r="U9" s="130" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="V9" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="W9" s="130"/>
       <c r="X9" s="130"/>
@@ -3494,10 +3564,31 @@
         <v>0</v>
       </c>
       <c r="AB9" s="115" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B10" s="102" t="s">
+        <v>372</v>
+      </c>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="103">
+        <f>SUM(E3:E9)</f>
+        <v>-4</v>
+      </c>
+      <c r="F10" s="104">
+        <f>SUM(F3:F9)</f>
+        <v>373197.01000000013</v>
+      </c>
+      <c r="G10" s="104">
+        <f>SUM(G3:G9)</f>
+        <v>340187.25999999995</v>
+      </c>
+      <c r="H10" s="104">
+        <f>SUM(H3:H9)</f>
+        <v>-33009.750000000007</v>
+      </c>
       <c r="J10" s="106" t="s">
         <v>43</v>
       </c>
@@ -3523,7 +3614,7 @@
         <v>0</v>
       </c>
       <c r="R10" s="143" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="S10" s="128">
         <f t="shared" si="3"/>
@@ -3533,11 +3624,11 @@
         <v>0.8</v>
       </c>
       <c r="U10" s="130" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="V10" s="130"/>
       <c r="W10" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="X10" s="130"/>
       <c r="Y10" s="128">
@@ -3553,7 +3644,7 @@
         <v>0</v>
       </c>
       <c r="AB10" s="115" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.3">
@@ -3582,7 +3673,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="143" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="S11" s="128">
         <f t="shared" si="3"/>
@@ -3592,11 +3683,11 @@
         <v>0.8</v>
       </c>
       <c r="U11" s="130" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="V11" s="130"/>
       <c r="W11" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="X11" s="130"/>
       <c r="Y11" s="128">
@@ -3612,12 +3703,10 @@
         <v>0</v>
       </c>
       <c r="AB11" s="115" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
-    <row r="12" spans="2:28" ht="40.799999999999997" x14ac:dyDescent="0.2">
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
+    <row r="12" spans="2:28" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="J12" s="106" t="s">
         <v>78</v>
       </c>
@@ -3638,14 +3727,14 @@
         <v>0</v>
       </c>
       <c r="P12" s="133" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="Q12" s="123">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R12" s="143" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="S12" s="128">
         <f t="shared" si="3"/>
@@ -3655,12 +3744,12 @@
         <v>0.8</v>
       </c>
       <c r="U12" s="130" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="V12" s="130"/>
       <c r="W12" s="130"/>
       <c r="X12" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="Y12" s="128">
         <f t="shared" si="5"/>
@@ -3675,7 +3764,7 @@
         <v>29220</v>
       </c>
       <c r="AB12" s="115" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="13" spans="2:28" ht="40.799999999999997" x14ac:dyDescent="0.2">
@@ -3701,14 +3790,14 @@
         <v>0</v>
       </c>
       <c r="P13" s="133" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="Q13" s="123">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R13" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S13" s="128">
         <f t="shared" si="3"/>
@@ -3734,7 +3823,7 @@
         <v>0</v>
       </c>
       <c r="AB13" s="115" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.2">
@@ -3765,7 +3854,7 @@
         <v>12531.68</v>
       </c>
       <c r="R14" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S14" s="128">
         <f t="shared" si="3"/>
@@ -3791,7 +3880,7 @@
         <v>0</v>
       </c>
       <c r="AB14" s="115" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="2:28" ht="30.6" x14ac:dyDescent="0.2">
@@ -3822,7 +3911,7 @@
         <v>12130.16</v>
       </c>
       <c r="R15" s="143" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="S15" s="128">
         <f t="shared" si="3"/>
@@ -3832,12 +3921,12 @@
         <v>1</v>
       </c>
       <c r="U15" s="130" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="V15" s="130"/>
       <c r="W15" s="130"/>
       <c r="X15" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="Y15" s="128">
         <f t="shared" si="5"/>
@@ -3852,12 +3941,12 @@
         <v>114077</v>
       </c>
       <c r="AB15" s="115" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="16" spans="2:28" ht="51" x14ac:dyDescent="0.2">
       <c r="D16" s="16"/>
-      <c r="E16" s="87"/>
+      <c r="E16" s="16"/>
       <c r="J16" s="106" t="s">
         <v>27</v>
       </c>
@@ -3878,14 +3967,14 @@
         <v>0</v>
       </c>
       <c r="P16" s="133" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="Q16" s="123">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R16" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S16" s="128">
         <f t="shared" si="3"/>
@@ -3911,7 +4000,7 @@
         <v>0</v>
       </c>
       <c r="AB16" s="115" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="17" spans="4:28" x14ac:dyDescent="0.2">
@@ -3942,7 +4031,7 @@
         <v>5268.24</v>
       </c>
       <c r="R17" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S17" s="128">
         <f t="shared" si="3"/>
@@ -3968,7 +4057,7 @@
         <v>0</v>
       </c>
       <c r="AB17" s="115" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="18" spans="4:28" x14ac:dyDescent="0.2">
@@ -3999,7 +4088,7 @@
         <v>8583.58</v>
       </c>
       <c r="R18" s="143" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="S18" s="128">
         <f t="shared" si="3"/>
@@ -4009,10 +4098,10 @@
         <v>0.03</v>
       </c>
       <c r="U18" s="130" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="V18" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="W18" s="130"/>
       <c r="X18" s="130"/>
@@ -4029,7 +4118,7 @@
         <v>0</v>
       </c>
       <c r="AB18" s="115" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="4:28" x14ac:dyDescent="0.2">
@@ -4060,7 +4149,7 @@
         <v>11224.67</v>
       </c>
       <c r="R19" s="143" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="S19" s="128">
         <f t="shared" si="3"/>
@@ -4070,10 +4159,10 @@
         <v>0.03</v>
       </c>
       <c r="U19" s="130" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="V19" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="W19" s="130"/>
       <c r="X19" s="130"/>
@@ -4090,7 +4179,7 @@
         <v>0</v>
       </c>
       <c r="AB19" s="115" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" spans="4:28" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -4121,7 +4210,7 @@
         <v>6910.4</v>
       </c>
       <c r="R20" s="143" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="S20" s="128">
         <f t="shared" si="3"/>
@@ -4131,11 +4220,11 @@
         <v>0.2</v>
       </c>
       <c r="U20" s="130" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="V20" s="130"/>
       <c r="W20" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="X20" s="130"/>
       <c r="Y20" s="128">
@@ -4151,14 +4240,14 @@
         <v>0</v>
       </c>
       <c r="AB20" s="115" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="21" spans="4:28" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="D21" s="16"/>
       <c r="E21" s="87"/>
       <c r="J21" s="106" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="K21" s="106" t="s">
         <v>94</v>
@@ -4182,7 +4271,7 @@
         <v>5595.2800000000007</v>
       </c>
       <c r="R21" s="143" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="S21" s="128">
         <f t="shared" si="3"/>
@@ -4192,11 +4281,11 @@
         <v>0.04</v>
       </c>
       <c r="U21" s="130" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="V21" s="130"/>
       <c r="W21" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="X21" s="130"/>
       <c r="Y21" s="128">
@@ -4212,7 +4301,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="115" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="22" spans="4:28" x14ac:dyDescent="0.2">
@@ -4243,7 +4332,7 @@
         <v>-6277.7</v>
       </c>
       <c r="R22" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S22" s="128">
         <f t="shared" si="3"/>
@@ -4253,12 +4342,12 @@
         <v>0.15</v>
       </c>
       <c r="U22" s="130" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="V22" s="130"/>
       <c r="W22" s="130"/>
       <c r="X22" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="Y22" s="128">
         <f t="shared" si="5"/>
@@ -4273,10 +4362,12 @@
         <v>6620.55</v>
       </c>
       <c r="AB22" s="115" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
-    <row r="23" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D23" s="16"/>
+      <c r="E23" s="87"/>
       <c r="J23" s="106" t="s">
         <v>72</v>
       </c>
@@ -4302,7 +4393,7 @@
         <v>-3984.32</v>
       </c>
       <c r="R23" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S23" s="128">
         <f t="shared" si="3"/>
@@ -4312,12 +4403,12 @@
         <v>0.15</v>
       </c>
       <c r="U23" s="130" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="V23" s="130"/>
       <c r="W23" s="130"/>
       <c r="X23" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="Y23" s="128">
         <f t="shared" si="5"/>
@@ -4332,7 +4423,7 @@
         <v>4200.5999999999995</v>
       </c>
       <c r="AB23" s="115" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="24" spans="4:28" ht="30.6" x14ac:dyDescent="0.3">
@@ -4346,7 +4437,7 @@
         <v>369</v>
       </c>
       <c r="M24" s="106" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="N24" s="123">
         <f t="shared" si="1"/>
@@ -4361,7 +4452,7 @@
         <v>-4289.12</v>
       </c>
       <c r="R24" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S24" s="128">
         <f t="shared" si="3"/>
@@ -4371,12 +4462,12 @@
         <v>0.15</v>
       </c>
       <c r="U24" s="130" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="V24" s="130"/>
       <c r="W24" s="130"/>
       <c r="X24" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="Y24" s="128">
         <f t="shared" si="5"/>
@@ -4391,7 +4482,7 @@
         <v>4430.8499999999995</v>
       </c>
       <c r="AB24" s="115" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="25" spans="4:28" x14ac:dyDescent="0.3">
@@ -4420,7 +4511,7 @@
         <v>-3509.2</v>
       </c>
       <c r="R25" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S25" s="128">
         <f t="shared" si="3"/>
@@ -4430,12 +4521,12 @@
         <v>0.15</v>
       </c>
       <c r="U25" s="130" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="V25" s="130"/>
       <c r="W25" s="130"/>
       <c r="X25" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="Y25" s="128">
         <f t="shared" si="5"/>
@@ -4450,7 +4541,7 @@
         <v>3084.75</v>
       </c>
       <c r="AB25" s="115" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="26" spans="4:28" x14ac:dyDescent="0.3">
@@ -4479,7 +4570,7 @@
         <v>-3442.4</v>
       </c>
       <c r="R26" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S26" s="128">
         <f t="shared" si="3"/>
@@ -4489,12 +4580,12 @@
         <v>0.15</v>
       </c>
       <c r="U26" s="130" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="V26" s="130"/>
       <c r="W26" s="130"/>
       <c r="X26" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="Y26" s="128">
         <f t="shared" si="5"/>
@@ -4509,7 +4600,7 @@
         <v>2959.5</v>
       </c>
       <c r="AB26" s="115" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="27" spans="4:28" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -4538,7 +4629,7 @@
         <v>-11204.91</v>
       </c>
       <c r="R27" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S27" s="128">
         <f t="shared" si="3"/>
@@ -4564,7 +4655,7 @@
         <v>0</v>
       </c>
       <c r="AB27" s="115" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="28" spans="4:28" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -4593,7 +4684,7 @@
         <v>-8685.7800000000007</v>
       </c>
       <c r="R28" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S28" s="128">
         <f t="shared" si="3"/>
@@ -4603,10 +4694,10 @@
         <v>0.15</v>
       </c>
       <c r="U28" s="130" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="V28" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="W28" s="130"/>
       <c r="X28" s="130"/>
@@ -4623,7 +4714,7 @@
         <v>0</v>
       </c>
       <c r="AB28" s="115" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="29" spans="4:28" x14ac:dyDescent="0.3">
@@ -4652,7 +4743,7 @@
         <v>-7348.7800000000007</v>
       </c>
       <c r="R29" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S29" s="128">
         <f t="shared" si="3"/>
@@ -4662,10 +4753,10 @@
         <v>0.15</v>
       </c>
       <c r="U29" s="130" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="V29" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="W29" s="130"/>
       <c r="X29" s="130"/>
@@ -4682,7 +4773,7 @@
         <v>0</v>
       </c>
       <c r="AB29" s="115" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="30" spans="4:28" x14ac:dyDescent="0.3">
@@ -4711,7 +4802,7 @@
         <v>-10697.49</v>
       </c>
       <c r="R30" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S30" s="128">
         <f t="shared" si="3"/>
@@ -4721,11 +4812,11 @@
         <v>0.15</v>
       </c>
       <c r="U30" s="130" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="V30" s="130"/>
       <c r="W30" s="130" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="X30" s="130"/>
       <c r="Y30" s="128">
@@ -4741,7 +4832,7 @@
         <v>0</v>
       </c>
       <c r="AB30" s="115" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="31" spans="4:28" ht="40.799999999999997" x14ac:dyDescent="0.3">
@@ -4765,14 +4856,14 @@
         <v>0</v>
       </c>
       <c r="P31" s="133" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="Q31" s="123">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R31" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S31" s="128">
         <f t="shared" si="3"/>
@@ -4798,7 +4889,7 @@
         <v>0</v>
       </c>
       <c r="AB31" s="115" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="32" spans="4:28" ht="40.799999999999997" x14ac:dyDescent="0.3">
@@ -4822,14 +4913,14 @@
         <v>0</v>
       </c>
       <c r="P32" s="133" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="Q32" s="123">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R32" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S32" s="128">
         <f t="shared" si="3"/>
@@ -4855,7 +4946,7 @@
         <v>0</v>
       </c>
       <c r="AB32" s="115" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="33" spans="10:28" ht="30.6" x14ac:dyDescent="0.3">
@@ -4879,14 +4970,14 @@
         <v>0</v>
       </c>
       <c r="P33" s="133" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="Q33" s="123">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R33" s="143" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S33" s="128">
         <f t="shared" si="3"/>
@@ -4912,7 +5003,7 @@
         <v>0</v>
       </c>
       <c r="AB33" s="115" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="34" spans="10:28" ht="30.6" x14ac:dyDescent="0.3">
@@ -4936,14 +5027,14 @@
         <v>0</v>
       </c>
       <c r="P34" s="134" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="Q34" s="125">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R34" s="144" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S34" s="129">
         <f t="shared" si="3"/>
@@ -4969,13 +5060,13 @@
         <v>0</v>
       </c>
       <c r="AB34" s="117" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="35" spans="10:28" x14ac:dyDescent="0.3">
       <c r="O35" s="122"/>
       <c r="P35" s="135" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="Q35" s="127">
         <f>SUM(Q4:Q34)</f>
@@ -4983,7 +5074,7 @@
       </c>
       <c r="R35" s="113"/>
       <c r="X35" s="142" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="Y35" s="132">
         <f>SUM(Y4:Y34)</f>
@@ -5000,7 +5091,7 @@
     </row>
     <row r="36" spans="10:28" x14ac:dyDescent="0.3">
       <c r="X36" s="142" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="Y36" s="132">
         <f>Y35/1</f>
@@ -5033,7 +5124,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z7" activeCellId="2" sqref="V7 X7 Z7"/>
+      <selection pane="bottomRight" activeCell="H27" sqref="H27:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -8710,7 +8801,7 @@
         <v>114</v>
       </c>
       <c r="H29" s="85" t="s">
-        <v>7</v>
+        <v>441</v>
       </c>
       <c r="I29" s="85" t="s">
         <v>369</v>
@@ -8831,7 +8922,7 @@
         <v>114</v>
       </c>
       <c r="H30" s="85" t="s">
-        <v>7</v>
+        <v>441</v>
       </c>
       <c r="I30" s="85" t="s">
         <v>369</v>
@@ -8952,10 +9043,10 @@
         <v>7</v>
       </c>
       <c r="H31" s="85" t="s">
-        <v>7</v>
+        <v>442</v>
       </c>
       <c r="I31" s="85" t="s">
-        <v>7</v>
+        <v>442</v>
       </c>
       <c r="J31" s="24" t="s">
         <v>1</v>
@@ -9073,10 +9164,10 @@
         <v>7</v>
       </c>
       <c r="H32" s="85" t="s">
-        <v>7</v>
-      </c>
-      <c r="I32" s="85" t="s">
-        <v>369</v>
+        <v>442</v>
+      </c>
+      <c r="I32" s="146" t="s">
+        <v>442</v>
       </c>
       <c r="J32" s="24" t="s">
         <v>1</v>
@@ -9194,7 +9285,7 @@
         <v>7</v>
       </c>
       <c r="H33" s="85" t="s">
-        <v>7</v>
+        <v>441</v>
       </c>
       <c r="I33" s="85" t="s">
         <v>369</v>
@@ -9315,7 +9406,7 @@
         <v>7</v>
       </c>
       <c r="H34" s="85" t="s">
-        <v>7</v>
+        <v>441</v>
       </c>
       <c r="I34" s="85" t="s">
         <v>369</v>
@@ -9436,7 +9527,7 @@
         <v>7</v>
       </c>
       <c r="H35" s="85" t="s">
-        <v>7</v>
+        <v>441</v>
       </c>
       <c r="I35" s="85" t="s">
         <v>369</v>
@@ -9657,16 +9748,16 @@
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C37" s="18" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E37" s="16" t="s">
         <v>113</v>
@@ -9684,10 +9775,10 @@
         <v>369</v>
       </c>
       <c r="J37" s="24" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="K37" s="30" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="L37" s="57" t="s">
         <v>193</v>
@@ -9797,8 +9888,8 @@
       <c r="H38" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="I38" s="86" t="s">
-        <v>369</v>
+      <c r="I38" s="146" t="s">
+        <v>363</v>
       </c>
       <c r="J38" s="24" t="s">
         <v>363</v>
@@ -9912,8 +10003,8 @@
       <c r="H39" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="I39" s="86" t="s">
-        <v>369</v>
+      <c r="I39" s="146" t="s">
+        <v>363</v>
       </c>
       <c r="J39" s="24" t="s">
         <v>363</v>
@@ -10027,8 +10118,8 @@
       <c r="H40" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="I40" s="86" t="s">
-        <v>369</v>
+      <c r="I40" s="146" t="s">
+        <v>363</v>
       </c>
       <c r="J40" s="24" t="s">
         <v>363</v>
@@ -10142,8 +10233,8 @@
       <c r="H41" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="I41" s="86" t="s">
-        <v>369</v>
+      <c r="I41" s="146" t="s">
+        <v>363</v>
       </c>
       <c r="J41" s="24" t="s">
         <v>363</v>
@@ -10893,7 +10984,7 @@
         <v>369</v>
       </c>
       <c r="I47" s="85" t="s">
-        <v>7</v>
+        <v>441</v>
       </c>
       <c r="J47" s="18" t="s">
         <v>1</v>
@@ -11024,7 +11115,7 @@
         <v>369</v>
       </c>
       <c r="I48" s="85" t="s">
-        <v>7</v>
+        <v>363</v>
       </c>
       <c r="J48" s="18" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
updates to some new & decommissioned sites
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20240409.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20240409.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4132169B-D6D4-4AE5-8DDC-F8DB022A1B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F242967-5349-4D3E-B662-7675B7D686DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Planning" sheetId="4" r:id="rId1"/>
@@ -2470,11 +2470,11 @@
     <xf numFmtId="44" fontId="5" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2905,9 +2905,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC6A41C-4EE9-4E25-91C6-882C326C1FB9}">
   <dimension ref="B2:AB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="10" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C3" sqref="C3"/>
+      <selection pane="topRight" activeCell="Q22" sqref="Q22:Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -2974,16 +2974,16 @@
       <c r="S2" s="140"/>
       <c r="T2" s="140"/>
       <c r="U2" s="140"/>
-      <c r="V2" s="145" t="s">
+      <c r="V2" s="146" t="s">
         <v>418</v>
       </c>
-      <c r="W2" s="145"/>
-      <c r="X2" s="145"/>
-      <c r="Y2" s="145" t="s">
+      <c r="W2" s="146"/>
+      <c r="X2" s="146"/>
+      <c r="Y2" s="146" t="s">
         <v>405</v>
       </c>
-      <c r="Z2" s="145"/>
-      <c r="AA2" s="145"/>
+      <c r="Z2" s="146"/>
+      <c r="AA2" s="146"/>
       <c r="AB2" s="136"/>
     </row>
     <row r="3" spans="2:28" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3001,7 +3001,7 @@
       </c>
       <c r="F3" s="94">
         <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B3,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>280203.16000000003</v>
+        <v>281421.40000000002</v>
       </c>
       <c r="G3" s="94">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B3,'O&amp;M Costs'!$AI$2:$AI$50)</f>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="H3" s="95">
         <f>G3-F3</f>
-        <v>17043.429999999993</v>
+        <v>15825.190000000002</v>
       </c>
       <c r="J3" s="89" t="s">
         <v>103</v>
@@ -3088,11 +3088,11 @@
       </c>
       <c r="G4" s="94">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B4,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>11204.91</v>
+        <v>12423.150000000001</v>
       </c>
       <c r="H4" s="95">
         <f t="shared" ref="H4:H8" si="0">G4-F4</f>
-        <v>-38533.42</v>
+        <v>-37315.18</v>
       </c>
       <c r="J4" s="106" t="s">
         <v>74</v>
@@ -3579,15 +3579,15 @@
       </c>
       <c r="F10" s="104">
         <f>SUM(F3:F9)</f>
-        <v>373197.01000000013</v>
+        <v>374415.25000000012</v>
       </c>
       <c r="G10" s="104">
         <f>SUM(G3:G9)</f>
-        <v>340187.25999999995</v>
+        <v>341405.50000000006</v>
       </c>
       <c r="H10" s="104">
         <f>SUM(H3:H9)</f>
-        <v>-33009.750000000007</v>
+        <v>-33009.749999999993</v>
       </c>
       <c r="J10" s="106" t="s">
         <v>43</v>
@@ -4618,7 +4618,7 @@
       </c>
       <c r="N27" s="123">
         <f t="shared" si="1"/>
-        <v>11204.91</v>
+        <v>12423.150000000001</v>
       </c>
       <c r="O27" s="124">
         <v>-1</v>
@@ -4626,14 +4626,14 @@
       <c r="P27" s="124"/>
       <c r="Q27" s="123">
         <f t="shared" si="2"/>
-        <v>-11204.91</v>
+        <v>-12423.150000000001</v>
       </c>
       <c r="R27" s="143" t="s">
         <v>374</v>
       </c>
       <c r="S27" s="128">
         <f t="shared" si="3"/>
-        <v>94259</v>
+        <v>80230</v>
       </c>
       <c r="T27" s="130"/>
       <c r="U27" s="130" t="s">
@@ -5070,7 +5070,7 @@
       </c>
       <c r="Q35" s="127">
         <f>SUM(Q4:Q34)</f>
-        <v>2804.3100000000013</v>
+        <v>1586.0700000000033</v>
       </c>
       <c r="R35" s="113"/>
       <c r="X35" s="142" t="s">
@@ -5120,11 +5120,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H27" sqref="H27:I28"/>
+      <selection pane="bottomRight" activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -9166,7 +9166,7 @@
       <c r="H32" s="85" t="s">
         <v>442</v>
       </c>
-      <c r="I32" s="146" t="s">
+      <c r="I32" s="145" t="s">
         <v>442</v>
       </c>
       <c r="J32" s="24" t="s">
@@ -9888,7 +9888,7 @@
       <c r="H38" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="I38" s="146" t="s">
+      <c r="I38" s="145" t="s">
         <v>363</v>
       </c>
       <c r="J38" s="24" t="s">
@@ -10003,7 +10003,7 @@
       <c r="H39" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="I39" s="146" t="s">
+      <c r="I39" s="145" t="s">
         <v>363</v>
       </c>
       <c r="J39" s="24" t="s">
@@ -10118,7 +10118,7 @@
       <c r="H40" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="I40" s="146" t="s">
+      <c r="I40" s="145" t="s">
         <v>363</v>
       </c>
       <c r="J40" s="24" t="s">
@@ -10233,7 +10233,7 @@
       <c r="H41" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="I41" s="146" t="s">
+      <c r="I41" s="145" t="s">
         <v>363</v>
       </c>
       <c r="J41" s="24" t="s">
@@ -11014,7 +11014,7 @@
       </c>
       <c r="Q47" s="17" t="str">
         <f t="shared" si="50"/>
-        <v>5060 Hybrid TEG</v>
+        <v>5120 TEG</v>
       </c>
       <c r="R47" s="16">
         <f t="shared" si="51"/>
@@ -11046,7 +11046,7 @@
       </c>
       <c r="Y47" s="19">
         <f t="shared" si="31"/>
-        <v>29303</v>
+        <v>15274</v>
       </c>
       <c r="Z47" s="19">
         <f t="shared" si="53"/>
@@ -11054,7 +11054,7 @@
       </c>
       <c r="AA47" s="20">
         <f t="shared" si="20"/>
-        <v>94259</v>
+        <v>80230</v>
       </c>
       <c r="AB47" s="39">
         <f t="shared" si="54"/>
@@ -11062,19 +11062,19 @@
       </c>
       <c r="AC47" s="20">
         <f t="shared" si="21"/>
-        <v>7540.72</v>
+        <v>6418.4000000000005</v>
       </c>
       <c r="AD47" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="AD47" si="55">(R47*battery_replacement)/4</f>
         <v>364</v>
       </c>
       <c r="AE47" s="21">
-        <f t="shared" si="33"/>
+        <f t="shared" ref="AE47" si="56">VLOOKUP(L47,communication,3,FALSE)</f>
         <v>1440</v>
       </c>
       <c r="AF47" s="21">
-        <f t="shared" si="34"/>
-        <v>780.19</v>
+        <f t="shared" ref="AF47" si="57">VLOOKUP(Q47,power,3,FALSE)</f>
+        <v>3120.75</v>
       </c>
       <c r="AG47" s="21">
         <f t="shared" si="25"/>
@@ -11082,11 +11082,11 @@
       </c>
       <c r="AH47" s="22">
         <f t="shared" si="23"/>
-        <v>3664.19</v>
+        <v>6004.75</v>
       </c>
       <c r="AI47" s="23">
         <f t="shared" si="22"/>
-        <v>11204.91</v>
+        <v>12423.150000000001</v>
       </c>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.2">
@@ -11548,31 +11548,31 @@
         <v>99</v>
       </c>
       <c r="T54" s="19">
-        <f t="shared" ref="T54:U57" si="55">SUMIFS(T$2:T$50,$D$2:$D$50,$S54,T$2:T$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="T54:U57" si="58">SUMIFS(T$2:T$50,$D$2:$D$50,$S54,T$2:T$50,"&lt;&gt;#N/A")</f>
         <v>39194</v>
       </c>
       <c r="U54" s="19">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>18370</v>
       </c>
       <c r="V54" s="19">
-        <f t="shared" ref="V54:Z54" si="56">SUMIFS(V$2:V$50,$D$2:$D$50,$S54,V$2:V$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="V54:Z54" si="59">SUMIFS(V$2:V$50,$D$2:$D$50,$S54,V$2:V$50,"&lt;&gt;#N/A")</f>
         <v>163900</v>
       </c>
       <c r="W54" s="19">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>206316</v>
       </c>
       <c r="X54" s="19">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>484275</v>
       </c>
       <c r="Y54" s="19">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>300581</v>
       </c>
       <c r="Z54" s="19">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>312500</v>
       </c>
       <c r="AA54" s="35">
@@ -11581,31 +11581,31 @@
       </c>
       <c r="AB54" s="35"/>
       <c r="AC54" s="35">
-        <f t="shared" ref="AC54:AE57" si="57">SUMIFS(AC$2:AC$50,$D$2:$D$50,$S54,AC$2:AC$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="AC54:AE57" si="60">SUMIFS(AC$2:AC$50,$D$2:$D$50,$S54,AC$2:AC$50,"&lt;&gt;#N/A")</f>
         <v>135396.36000000002</v>
       </c>
       <c r="AD54" s="21">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>9282</v>
       </c>
       <c r="AE54" s="21">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>26580</v>
       </c>
       <c r="AF54" s="21">
-        <f t="shared" ref="AF54:AG54" si="58">SUMIFS(AF$2:AF$50,$D$2:$D$50,$S54,AF$2:AF$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="AF54:AG54" si="61">SUMIFS(AF$2:AF$50,$D$2:$D$50,$S54,AF$2:AF$50,"&lt;&gt;#N/A")</f>
         <v>22505.100000000002</v>
       </c>
       <c r="AG54" s="21">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>27000</v>
       </c>
       <c r="AH54" s="36">
-        <f t="shared" ref="AH54:AI57" si="59">SUMIFS(AH$2:AH$50,$D$2:$D$50,$S54,AH$2:AH$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="AH54:AI57" si="62">SUMIFS(AH$2:AH$50,$D$2:$D$50,$S54,AH$2:AH$50,"&lt;&gt;#N/A")</f>
         <v>85367.1</v>
       </c>
       <c r="AI54" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>220763.45999999996</v>
       </c>
     </row>
@@ -11614,31 +11614,31 @@
         <v>94</v>
       </c>
       <c r="T55" s="19">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>13142</v>
       </c>
       <c r="U55" s="19">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>7515</v>
       </c>
       <c r="V55" s="19">
-        <f t="shared" ref="V55:Z57" si="60">SUMIFS(V$2:V$50,$D$2:$D$50,$S55,V$2:V$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="V55:Z57" si="63">SUMIFS(V$2:V$50,$D$2:$D$50,$S55,V$2:V$50,"&lt;&gt;#N/A")</f>
         <v>44100</v>
       </c>
       <c r="W55" s="19">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>156300</v>
       </c>
       <c r="X55" s="19">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>231865</v>
       </c>
       <c r="Y55" s="19">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>69606</v>
       </c>
       <c r="Z55" s="19">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>112500</v>
       </c>
       <c r="AA55" s="35">
@@ -11647,31 +11647,31 @@
       </c>
       <c r="AB55" s="35"/>
       <c r="AC55" s="35">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>51532.739999999991</v>
       </c>
       <c r="AD55" s="21">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>2912</v>
       </c>
       <c r="AE55" s="21">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>8940</v>
       </c>
       <c r="AF55" s="21">
-        <f t="shared" ref="AF55:AG57" si="61">SUMIFS(AF$2:AF$50,$D$2:$D$50,$S55,AF$2:AF$50,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="AF55:AG57" si="64">SUMIFS(AF$2:AF$50,$D$2:$D$50,$S55,AF$2:AF$50,"&lt;&gt;#N/A")</f>
         <v>6841.51</v>
       </c>
       <c r="AG55" s="21">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>9720</v>
       </c>
       <c r="AH55" s="36">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>28413.510000000002</v>
       </c>
       <c r="AI55" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>79946.25</v>
       </c>
     </row>
@@ -11680,31 +11680,31 @@
         <v>97</v>
       </c>
       <c r="T56" s="19">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>6742</v>
       </c>
       <c r="U56" s="19">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>3340</v>
       </c>
       <c r="V56" s="19">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>17800</v>
       </c>
       <c r="W56" s="19">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>83360</v>
       </c>
       <c r="X56" s="19">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>117400</v>
       </c>
       <c r="Y56" s="19">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>63801</v>
       </c>
       <c r="Z56" s="19">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>50000</v>
       </c>
       <c r="AA56" s="35">
@@ -11713,31 +11713,31 @@
       </c>
       <c r="AB56" s="35"/>
       <c r="AC56" s="35">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>27395.439999999999</v>
       </c>
       <c r="AD56" s="21">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>1456</v>
       </c>
       <c r="AE56" s="21">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>4620</v>
       </c>
       <c r="AF56" s="21">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>7141.6900000000005</v>
       </c>
       <c r="AG56" s="21">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>4320</v>
       </c>
       <c r="AH56" s="36">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>17537.690000000002</v>
       </c>
       <c r="AI56" s="37">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>44933.13</v>
       </c>
     </row>
@@ -11746,65 +11746,65 @@
         <v>98</v>
       </c>
       <c r="T57" s="19">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>11710</v>
       </c>
       <c r="U57" s="19">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>5845</v>
       </c>
       <c r="V57" s="19">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>38450</v>
       </c>
       <c r="W57" s="19">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>35428</v>
       </c>
       <c r="X57" s="19">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>99790</v>
       </c>
       <c r="Y57" s="19">
-        <f t="shared" si="60"/>
-        <v>117262</v>
+        <f t="shared" si="63"/>
+        <v>103233</v>
       </c>
       <c r="Z57" s="19">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>75000</v>
       </c>
       <c r="AA57" s="35">
         <f>SUMIFS(AA$2:AA$50,$D$2:$D$50,$S57,AA$2:AA$50,"&lt;&gt;#N/A")</f>
-        <v>383485</v>
+        <v>369456</v>
       </c>
       <c r="AB57" s="35"/>
       <c r="AC57" s="35">
-        <f t="shared" si="57"/>
-        <v>34506.560000000005</v>
+        <f t="shared" si="60"/>
+        <v>33384.240000000005</v>
       </c>
       <c r="AD57" s="21">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>2912</v>
       </c>
       <c r="AE57" s="21">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>7260</v>
       </c>
       <c r="AF57" s="21">
-        <f t="shared" si="61"/>
-        <v>5041.1400000000012</v>
+        <f t="shared" si="64"/>
+        <v>7381.7000000000007</v>
       </c>
       <c r="AG57" s="21">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>9720</v>
       </c>
       <c r="AH57" s="36">
-        <f t="shared" si="59"/>
-        <v>24933.14</v>
+        <f t="shared" si="62"/>
+        <v>27273.7</v>
       </c>
       <c r="AI57" s="37">
-        <f t="shared" si="59"/>
-        <v>59439.7</v>
+        <f t="shared" si="62"/>
+        <v>60657.939999999995</v>
       </c>
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.2">
@@ -11816,37 +11816,37 @@
         <v>50904</v>
       </c>
       <c r="U59" s="47">
-        <f t="shared" ref="U59:AG59" si="62">U54+U57</f>
+        <f t="shared" ref="U59:AG59" si="65">U54+U57</f>
         <v>24215</v>
       </c>
       <c r="V59" s="47">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>202350</v>
       </c>
       <c r="W59" s="47">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>241744</v>
       </c>
       <c r="X59" s="47">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>584065</v>
       </c>
       <c r="Y59" s="47">
-        <f t="shared" si="62"/>
-        <v>417843</v>
+        <f t="shared" si="65"/>
+        <v>403814</v>
       </c>
       <c r="Z59" s="47">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>387500</v>
       </c>
       <c r="AA59" s="48">
         <f>AA54+AA57</f>
-        <v>1908621</v>
+        <v>1894592</v>
       </c>
       <c r="AB59" s="48"/>
       <c r="AC59" s="48">
         <f>AC54+AC57</f>
-        <v>169902.92</v>
+        <v>168780.60000000003</v>
       </c>
       <c r="AD59" s="49">
         <f>AD54+AD57</f>
@@ -11857,20 +11857,20 @@
         <v>33840</v>
       </c>
       <c r="AF59" s="49">
-        <f t="shared" si="62"/>
-        <v>27546.240000000005</v>
+        <f t="shared" si="65"/>
+        <v>29886.800000000003</v>
       </c>
       <c r="AG59" s="49">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>36720</v>
       </c>
       <c r="AH59" s="50">
         <f>AH54+AH57</f>
-        <v>110300.24</v>
+        <v>112640.8</v>
       </c>
       <c r="AI59" s="51">
         <f>AI54+AI57</f>
-        <v>280203.15999999997</v>
+        <v>281421.39999999997</v>
       </c>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.2">
@@ -11882,27 +11882,27 @@
         <v>59078</v>
       </c>
       <c r="U60" s="47">
-        <f t="shared" ref="U60:AG60" si="63">SUM(U54:U56)</f>
+        <f t="shared" ref="U60:AG60" si="66">SUM(U54:U56)</f>
         <v>29225</v>
       </c>
       <c r="V60" s="47">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>225800</v>
       </c>
       <c r="W60" s="47">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>445976</v>
       </c>
       <c r="X60" s="47">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>833540</v>
       </c>
       <c r="Y60" s="47">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>433988</v>
       </c>
       <c r="Z60" s="47">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>475000</v>
       </c>
       <c r="AA60" s="48">
@@ -11919,15 +11919,15 @@
         <v>13650</v>
       </c>
       <c r="AE60" s="49">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>40140</v>
       </c>
       <c r="AF60" s="49">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>36488.300000000003</v>
       </c>
       <c r="AG60" s="49">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>41040</v>
       </c>
       <c r="AH60" s="50">
@@ -11948,61 +11948,61 @@
         <v>8174</v>
       </c>
       <c r="U61" s="47">
-        <f t="shared" ref="U61:AG61" si="64">U60-U59</f>
+        <f t="shared" ref="U61:AG61" si="67">U60-U59</f>
         <v>5010</v>
       </c>
       <c r="V61" s="47">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>23450</v>
       </c>
       <c r="W61" s="47">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>204232</v>
       </c>
       <c r="X61" s="47">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>249475</v>
       </c>
       <c r="Y61" s="47">
-        <f t="shared" si="64"/>
-        <v>16145</v>
+        <f t="shared" si="67"/>
+        <v>30174</v>
       </c>
       <c r="Z61" s="47">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>87500</v>
       </c>
       <c r="AA61" s="48">
         <f>AA60-AA59</f>
-        <v>593986</v>
+        <v>608015</v>
       </c>
       <c r="AB61" s="48"/>
       <c r="AC61" s="48">
         <f>AC60-AC59</f>
-        <v>44421.619999999995</v>
+        <v>45543.939999999973</v>
       </c>
       <c r="AD61" s="49">
         <f>AD60-AD59</f>
         <v>1456</v>
       </c>
       <c r="AE61" s="49">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>6300</v>
       </c>
       <c r="AF61" s="49">
-        <f t="shared" si="64"/>
-        <v>8942.0599999999977</v>
+        <f t="shared" si="67"/>
+        <v>6601.5</v>
       </c>
       <c r="AG61" s="49">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>4320</v>
       </c>
       <c r="AH61" s="50">
         <f>AH60-AH59</f>
-        <v>21018.060000000012</v>
+        <v>18677.500000000015</v>
       </c>
       <c r="AI61" s="51">
         <f>AI60-AI59</f>
-        <v>65439.679999999993</v>
+        <v>64221.440000000002</v>
       </c>
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.2">
@@ -12014,61 +12014,61 @@
         <v>0.16057677196291056</v>
       </c>
       <c r="U62" s="52">
-        <f t="shared" ref="U62:AG62" si="65">U61/U59</f>
+        <f t="shared" ref="U62:AG62" si="68">U61/U59</f>
         <v>0.20689655172413793</v>
       </c>
       <c r="V62" s="52">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>0.11588831233012108</v>
       </c>
       <c r="W62" s="52">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>0.84482758620689657</v>
       </c>
       <c r="X62" s="52">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>0.42713567839195982</v>
       </c>
       <c r="Y62" s="52">
-        <f t="shared" si="65"/>
-        <v>3.863891461625539E-2</v>
+        <f t="shared" si="68"/>
+        <v>7.47225207645104E-2</v>
       </c>
       <c r="Z62" s="52">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>0.22580645161290322</v>
       </c>
       <c r="AA62" s="53">
         <f>AA61/AA59</f>
-        <v>0.31121212645150609</v>
+        <v>0.32092133820896529</v>
       </c>
       <c r="AB62" s="53"/>
       <c r="AC62" s="53">
         <f>AC61/AC59</f>
-        <v>0.26145295207404318</v>
+        <v>0.26984108363164938</v>
       </c>
       <c r="AD62" s="54">
         <f>AD61/AD59</f>
         <v>0.11940298507462686</v>
       </c>
       <c r="AE62" s="54">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>0.18617021276595744</v>
       </c>
       <c r="AF62" s="54">
-        <f t="shared" si="65"/>
-        <v>0.32461998443344703</v>
+        <f t="shared" si="68"/>
+        <v>0.22088346694861943</v>
       </c>
       <c r="AG62" s="54">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="AH62" s="55">
         <f>AH61/AH59</f>
-        <v>0.19055316652076199</v>
+        <v>0.16581469591835299</v>
       </c>
       <c r="AI62" s="56">
         <f>AI61/AI59</f>
-        <v>0.23354369022819013</v>
+        <v>0.22820382529544664</v>
       </c>
     </row>
   </sheetData>
@@ -12087,7 +12087,7 @@
   <dimension ref="A1:AW47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AW1"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -14672,7 +14672,7 @@
         <v>-115.579713</v>
       </c>
       <c r="I19" s="64" t="s">
-        <v>183</v>
+        <v>230</v>
       </c>
       <c r="J19" s="64" t="s">
         <v>184</v>

</xml_diff>

<commit_message>
added cost estimates for SFG
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20240409.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20240409.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F242967-5349-4D3E-B662-7675B7D686DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68891CC-DBFF-46A9-B8CA-42168B20258D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Planning" sheetId="4" r:id="rId1"/>
@@ -57,6 +57,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Mike Ackerman</author>
+    <author>tc={F019DFCD-6A77-4755-B26D-65DA457FD8E0}</author>
+    <author>tc={52FFB650-6549-4688-8A3F-7A780B0AB6F2}</author>
+    <author>tc={6478D133-41BE-4FC3-816D-3C67573C708B}</author>
     <author>tc={010A182B-A551-4254-B23A-44D962FA2B27}</author>
   </authors>
   <commentList>
@@ -88,7 +91,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q35" authorId="1" shapeId="0" xr:uid="{010A182B-A551-4254-B23A-44D962FA2B27}">
+    <comment ref="D8" authorId="1" shapeId="0" xr:uid="{F019DFCD-6A77-4755-B26D-65DA457FD8E0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    SBT could consider moving YFK and PCA to IPTDS O&amp;M with funds.</t>
+      </text>
+    </comment>
+    <comment ref="M12" authorId="2" shapeId="0" xr:uid="{52FFB650-6549-4688-8A3F-7A780B0AB6F2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Could be moved to IPTDS O&amp;M with funds.</t>
+      </text>
+    </comment>
+    <comment ref="M13" authorId="3" shapeId="0" xr:uid="{6478D133-41BE-4FC3-816D-3C67573C708B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Could be moved to IPTDS O&amp;M with funds.</t>
+      </text>
+    </comment>
+    <comment ref="Q35" authorId="4" shapeId="0" xr:uid="{010A182B-A551-4254-B23A-44D962FA2B27}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -461,7 +488,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2133" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2136" uniqueCount="443">
   <si>
     <t>WDFW</t>
   </si>
@@ -1588,9 +1615,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>YFK, PCA</t>
-  </si>
-  <si>
     <t>CAC, BTL, LLS, BHC</t>
   </si>
   <si>
@@ -1778,9 +1802,6 @@
   </si>
   <si>
     <t>Ideally, site evaluations would occur in 2025 with installation in 2026 or 2027.</t>
-  </si>
-  <si>
-    <t>PCA, YFK, SW1, SW2, LAP, WR2, MR1, WEN, ACM</t>
   </si>
   <si>
     <t>SW1, SW2, LAP, WR2, MR1</t>
@@ -1831,6 +1852,9 @@
       </rPr>
       <t>, IR2</t>
     </r>
+  </si>
+  <si>
+    <t>SW1, SW2, LAP, WR2, MR1, WEN, ACM</t>
   </si>
 </sst>
 </file>
@@ -2773,6 +2797,15 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D8" dT="2025-08-06T20:39:50.78" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{F019DFCD-6A77-4755-B26D-65DA457FD8E0}">
+    <text>SBT could consider moving YFK and PCA to IPTDS O&amp;M with funds.</text>
+  </threadedComment>
+  <threadedComment ref="M12" dT="2025-08-06T21:07:49.41" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{52FFB650-6549-4688-8A3F-7A780B0AB6F2}">
+    <text>Could be moved to IPTDS O&amp;M with funds.</text>
+  </threadedComment>
+  <threadedComment ref="M13" dT="2025-08-06T21:08:00.50" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{6478D133-41BE-4FC3-816D-3C67573C708B}">
+    <text>Could be moved to IPTDS O&amp;M with funds.</text>
+  </threadedComment>
   <threadedComment ref="Q35" dT="2025-07-24T14:41:36.33" personId="{C77DAA69-426B-4B66-A041-374F39380B56}" id="{010A182B-A551-4254-B23A-44D962FA2B27}">
     <text>Difference btw this amount &amp; cell H3 is equal to O&amp;M costs for YFK, PCA.</text>
   </threadedComment>
@@ -2905,9 +2938,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC6A41C-4EE9-4E25-91C6-882C326C1FB9}">
   <dimension ref="B2:AB36"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="10" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q22" sqref="Q22:Q30"/>
+      <selection pane="topRight" activeCell="B12" sqref="B12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -2922,8 +2955,7 @@
     <col min="9" max="9" width="1.77734375" style="96" customWidth="1"/>
     <col min="10" max="10" width="11.88671875" style="96" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="33.77734375" style="96" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.44140625" style="96" customWidth="1"/>
-    <col min="13" max="13" width="10.21875" style="96" customWidth="1"/>
+    <col min="12" max="13" width="12.21875" style="96" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.88671875" style="96" customWidth="1"/>
     <col min="15" max="15" width="5.5546875" style="96" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.77734375" style="96" customWidth="1"/>
@@ -2945,22 +2977,22 @@
         <v>371</v>
       </c>
       <c r="C2" s="119" t="s">
+        <v>384</v>
+      </c>
+      <c r="D2" s="119" t="s">
         <v>385</v>
-      </c>
-      <c r="D2" s="119" t="s">
-        <v>386</v>
       </c>
       <c r="E2" s="121" t="s">
         <v>373</v>
       </c>
       <c r="F2" s="118" t="s">
+        <v>376</v>
+      </c>
+      <c r="G2" s="118" t="s">
         <v>377</v>
       </c>
-      <c r="G2" s="118" t="s">
+      <c r="H2" s="118" t="s">
         <v>378</v>
-      </c>
-      <c r="H2" s="118" t="s">
-        <v>379</v>
       </c>
       <c r="J2" s="136"/>
       <c r="K2" s="136"/>
@@ -2975,12 +3007,12 @@
       <c r="T2" s="140"/>
       <c r="U2" s="140"/>
       <c r="V2" s="146" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="W2" s="146"/>
       <c r="X2" s="146"/>
       <c r="Y2" s="146" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Z2" s="146"/>
       <c r="AA2" s="146"/>
@@ -2991,13 +3023,13 @@
         <v>369</v>
       </c>
       <c r="C3" s="92" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E3" s="93">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F3" s="94">
         <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B3,'O&amp;M Costs'!$AI$2:$AI$50)</f>
@@ -3005,11 +3037,11 @@
       </c>
       <c r="G3" s="94">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B3,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>297246.59000000003</v>
+        <v>283007.46999999997</v>
       </c>
       <c r="H3" s="95">
         <f>G3-F3</f>
-        <v>15825.190000000002</v>
+        <v>1586.0699999999488</v>
       </c>
       <c r="J3" s="89" t="s">
         <v>103</v>
@@ -3021,66 +3053,66 @@
         <v>367</v>
       </c>
       <c r="M3" s="89" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="N3" s="137" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O3" s="137" t="s">
+        <v>400</v>
+      </c>
+      <c r="P3" s="137" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q3" s="137" t="s">
+        <v>402</v>
+      </c>
+      <c r="R3" s="138" t="s">
+        <v>388</v>
+      </c>
+      <c r="S3" s="138" t="s">
         <v>401</v>
       </c>
-      <c r="P3" s="137" t="s">
-        <v>406</v>
-      </c>
-      <c r="Q3" s="137" t="s">
-        <v>403</v>
-      </c>
-      <c r="R3" s="138" t="s">
-        <v>389</v>
-      </c>
-      <c r="S3" s="138" t="s">
-        <v>402</v>
-      </c>
       <c r="T3" s="138" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="U3" s="138" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="V3" s="138">
         <v>2025</v>
       </c>
       <c r="W3" s="138" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="X3" s="138" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Y3" s="138">
         <v>2025</v>
       </c>
       <c r="Z3" s="138" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AA3" s="138" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="AB3" s="88" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="91" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C4" s="92" t="s">
-        <v>47</v>
+        <v>374</v>
       </c>
       <c r="D4" s="92" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E4" s="93">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="F4" s="94">
         <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B4,'O&amp;M Costs'!$AI$2:$AI$50)</f>
@@ -3088,11 +3120,11 @@
       </c>
       <c r="G4" s="94">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B4,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>12423.150000000001</v>
+        <v>0</v>
       </c>
       <c r="H4" s="95">
-        <f t="shared" ref="H4:H8" si="0">G4-F4</f>
-        <v>-37315.18</v>
+        <f t="shared" ref="H4:H9" si="0">G4-F4</f>
+        <v>-49738.33</v>
       </c>
       <c r="J4" s="106" t="s">
         <v>74</v>
@@ -3119,7 +3151,7 @@
         <v>0</v>
       </c>
       <c r="R4" s="143" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="S4" s="128">
         <f t="shared" ref="S4:S34" si="3">VLOOKUP(J4,om_costs,27,FALSE)</f>
@@ -3129,11 +3161,11 @@
         <v>0.8</v>
       </c>
       <c r="U4" s="130" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="V4" s="130"/>
       <c r="W4" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="X4" s="130"/>
       <c r="Y4" s="128">
@@ -3154,7 +3186,7 @@
     </row>
     <row r="5" spans="2:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="91" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C5" s="92" t="s">
         <v>374</v>
@@ -3202,7 +3234,7 @@
         <v>0</v>
       </c>
       <c r="R5" s="143" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="S5" s="128">
         <f t="shared" si="3"/>
@@ -3212,10 +3244,10 @@
         <v>0.8</v>
       </c>
       <c r="U5" s="130" t="s">
+        <v>411</v>
+      </c>
+      <c r="V5" s="130" t="s">
         <v>412</v>
-      </c>
-      <c r="V5" s="130" t="s">
-        <v>413</v>
       </c>
       <c r="W5" s="130"/>
       <c r="X5" s="130"/>
@@ -3232,33 +3264,33 @@
         <v>0</v>
       </c>
       <c r="AB5" s="115" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="91" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C6" s="92" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="92" t="s">
         <v>374</v>
       </c>
-      <c r="D6" s="92" t="s">
-        <v>34</v>
-      </c>
       <c r="E6" s="93">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F6" s="94">
         <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B6,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>6910.4</v>
+        <v>0</v>
       </c>
       <c r="G6" s="94">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B6,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>0</v>
+        <v>12423.150000000001</v>
       </c>
       <c r="H6" s="95">
         <f t="shared" si="0"/>
-        <v>-6910.4</v>
+        <v>12423.150000000001</v>
       </c>
       <c r="J6" s="106" t="s">
         <v>15</v>
@@ -3285,7 +3317,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="143" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="S6" s="128">
         <f t="shared" si="3"/>
@@ -3295,11 +3327,11 @@
         <v>1</v>
       </c>
       <c r="U6" s="130" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="V6" s="130"/>
       <c r="W6" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="X6" s="130"/>
       <c r="Y6" s="128">
@@ -3315,25 +3347,25 @@
         <v>0</v>
       </c>
       <c r="AB6" s="115" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="2:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="91" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C7" s="92" t="s">
         <v>374</v>
       </c>
       <c r="D7" s="92" t="s">
-        <v>375</v>
+        <v>34</v>
       </c>
       <c r="E7" s="93">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="F7" s="94">
         <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B7,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>14239.119999999999</v>
+        <v>6910.4</v>
       </c>
       <c r="G7" s="94">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B7,'O&amp;M Costs'!$AI$2:$AI$50)</f>
@@ -3341,7 +3373,7 @@
       </c>
       <c r="H7" s="95">
         <f t="shared" si="0"/>
-        <v>-14239.119999999999</v>
+        <v>-6910.4</v>
       </c>
       <c r="J7" s="106" t="s">
         <v>9</v>
@@ -3368,7 +3400,7 @@
         <v>0</v>
       </c>
       <c r="R7" s="143" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="S7" s="128">
         <f t="shared" si="3"/>
@@ -3378,12 +3410,12 @@
         <v>0.8</v>
       </c>
       <c r="U7" s="130" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="V7" s="130"/>
       <c r="W7" s="130"/>
       <c r="X7" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="Y7" s="128">
         <f t="shared" si="5"/>
@@ -3402,29 +3434,29 @@
       </c>
     </row>
     <row r="8" spans="2:28" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B8" s="107" t="s">
-        <v>370</v>
-      </c>
-      <c r="C8" s="108" t="s">
-        <v>376</v>
-      </c>
-      <c r="D8" s="108" t="s">
+      <c r="B8" s="91" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="92" t="s">
         <v>374</v>
       </c>
-      <c r="E8" s="109">
-        <v>4</v>
-      </c>
-      <c r="F8" s="110">
+      <c r="D8" s="92" t="s">
+        <v>374</v>
+      </c>
+      <c r="E8" s="93">
+        <v>0</v>
+      </c>
+      <c r="F8" s="94">
         <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B8,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="110">
+        <v>14239.119999999999</v>
+      </c>
+      <c r="G8" s="94">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B8,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>15225.039999999999</v>
-      </c>
-      <c r="H8" s="111">
+        <v>14239.119999999999</v>
+      </c>
+      <c r="H8" s="95">
         <f t="shared" si="0"/>
-        <v>15225.039999999999</v>
+        <v>0</v>
       </c>
       <c r="J8" s="106" t="s">
         <v>11</v>
@@ -3451,7 +3483,7 @@
         <v>0</v>
       </c>
       <c r="R8" s="143" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="S8" s="128">
         <f t="shared" si="3"/>
@@ -3461,12 +3493,12 @@
         <v>0.25</v>
       </c>
       <c r="U8" s="130" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="V8" s="130"/>
       <c r="W8" s="130"/>
       <c r="X8" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="Y8" s="128">
         <f t="shared" si="5"/>
@@ -3481,33 +3513,33 @@
         <v>16394.5</v>
       </c>
       <c r="AB8" s="115" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="9" spans="2:28" s="105" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="98" t="s">
+      <c r="B9" s="107" t="s">
+        <v>370</v>
+      </c>
+      <c r="C9" s="108" t="s">
+        <v>375</v>
+      </c>
+      <c r="D9" s="108" t="s">
         <v>374</v>
       </c>
-      <c r="D9" s="98" t="s">
-        <v>380</v>
-      </c>
-      <c r="E9" s="99">
-        <v>-1</v>
-      </c>
-      <c r="F9" s="100">
+      <c r="E9" s="109">
+        <v>4</v>
+      </c>
+      <c r="F9" s="110">
         <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B9,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>5595.2800000000007</v>
-      </c>
-      <c r="G9" s="100">
+        <v>0</v>
+      </c>
+      <c r="G9" s="110">
         <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B9,'O&amp;M Costs'!$AI$2:$AI$50)</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="101">
-        <f t="shared" ref="H9" si="8">G9-F9</f>
-        <v>-5595.2800000000007</v>
+        <v>15225.039999999999</v>
+      </c>
+      <c r="H9" s="111">
+        <f t="shared" si="0"/>
+        <v>15225.039999999999</v>
       </c>
       <c r="J9" s="106" t="s">
         <v>86</v>
@@ -3534,7 +3566,7 @@
         <v>0</v>
       </c>
       <c r="R9" s="143" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="S9" s="128">
         <f t="shared" si="3"/>
@@ -3544,10 +3576,10 @@
         <v>0.8</v>
       </c>
       <c r="U9" s="130" t="s">
+        <v>411</v>
+      </c>
+      <c r="V9" s="130" t="s">
         <v>412</v>
-      </c>
-      <c r="V9" s="130" t="s">
-        <v>413</v>
       </c>
       <c r="W9" s="130"/>
       <c r="X9" s="130"/>
@@ -3564,30 +3596,33 @@
         <v>0</v>
       </c>
       <c r="AB9" s="115" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B10" s="102" t="s">
-        <v>372</v>
-      </c>
-      <c r="C10" s="90"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="103">
-        <f>SUM(E3:E9)</f>
-        <v>-4</v>
-      </c>
-      <c r="F10" s="104">
-        <f>SUM(F3:F9)</f>
-        <v>374415.25000000012</v>
-      </c>
-      <c r="G10" s="104">
-        <f>SUM(G3:G9)</f>
-        <v>341405.50000000006</v>
-      </c>
-      <c r="H10" s="104">
-        <f>SUM(H3:H9)</f>
-        <v>-33009.749999999993</v>
+      <c r="B10" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="98" t="s">
+        <v>374</v>
+      </c>
+      <c r="D10" s="98" t="s">
+        <v>379</v>
+      </c>
+      <c r="E10" s="99">
+        <v>-1</v>
+      </c>
+      <c r="F10" s="100">
+        <f>SUMIF('O&amp;M Costs'!$H$2:$H$50,B10,'O&amp;M Costs'!$AI$2:$AI$50)</f>
+        <v>5595.2800000000007</v>
+      </c>
+      <c r="G10" s="100">
+        <f>SUMIF('O&amp;M Costs'!$I$2:$I$50,B10,'O&amp;M Costs'!$AI$2:$AI$50)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="101">
+        <f t="shared" ref="H10" si="8">G10-F10</f>
+        <v>-5595.2800000000007</v>
       </c>
       <c r="J10" s="106" t="s">
         <v>43</v>
@@ -3614,7 +3649,7 @@
         <v>0</v>
       </c>
       <c r="R10" s="143" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="S10" s="128">
         <f t="shared" si="3"/>
@@ -3624,11 +3659,11 @@
         <v>0.8</v>
       </c>
       <c r="U10" s="130" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="V10" s="130"/>
       <c r="W10" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="X10" s="130"/>
       <c r="Y10" s="128">
@@ -3648,6 +3683,27 @@
       </c>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B11" s="102" t="s">
+        <v>372</v>
+      </c>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="103">
+        <f>SUM(E3:E10)</f>
+        <v>-4</v>
+      </c>
+      <c r="F11" s="104">
+        <f>SUM(F3:F10)</f>
+        <v>374415.25000000012</v>
+      </c>
+      <c r="G11" s="104">
+        <f>SUM(G3:G10)</f>
+        <v>341405.49999999994</v>
+      </c>
+      <c r="H11" s="104">
+        <f>SUM(H3:H10)</f>
+        <v>-33009.750000000051</v>
+      </c>
       <c r="J11" s="106" t="s">
         <v>37</v>
       </c>
@@ -3673,7 +3729,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="143" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="S11" s="128">
         <f t="shared" si="3"/>
@@ -3683,11 +3739,11 @@
         <v>0.8</v>
       </c>
       <c r="U11" s="130" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="V11" s="130"/>
       <c r="W11" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="X11" s="130"/>
       <c r="Y11" s="128">
@@ -3717,7 +3773,7 @@
         <v>53</v>
       </c>
       <c r="M12" s="106" t="s">
-        <v>369</v>
+        <v>53</v>
       </c>
       <c r="N12" s="123">
         <f t="shared" si="1"/>
@@ -3727,14 +3783,14 @@
         <v>0</v>
       </c>
       <c r="P12" s="133" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q12" s="123">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R12" s="143" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="S12" s="128">
         <f t="shared" si="3"/>
@@ -3744,12 +3800,12 @@
         <v>0.8</v>
       </c>
       <c r="U12" s="130" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="V12" s="130"/>
       <c r="W12" s="130"/>
       <c r="X12" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="Y12" s="128">
         <f t="shared" si="5"/>
@@ -3764,12 +3820,10 @@
         <v>29220</v>
       </c>
       <c r="AB12" s="115" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
-    <row r="13" spans="2:28" ht="40.799999999999997" x14ac:dyDescent="0.2">
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
+    <row r="13" spans="2:28" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="J13" s="106" t="s">
         <v>56</v>
       </c>
@@ -3780,7 +3834,7 @@
         <v>53</v>
       </c>
       <c r="M13" s="106" t="s">
-        <v>369</v>
+        <v>53</v>
       </c>
       <c r="N13" s="123">
         <f t="shared" si="1"/>
@@ -3790,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="133" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q13" s="123">
         <f t="shared" si="2"/>
@@ -3823,7 +3877,7 @@
         <v>0</v>
       </c>
       <c r="AB13" s="115" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.2">
@@ -3836,7 +3890,7 @@
         <v>94</v>
       </c>
       <c r="L14" s="106" t="s">
-        <v>7</v>
+        <v>439</v>
       </c>
       <c r="M14" s="106" t="s">
         <v>369</v>
@@ -3893,7 +3947,7 @@
         <v>94</v>
       </c>
       <c r="L15" s="106" t="s">
-        <v>7</v>
+        <v>439</v>
       </c>
       <c r="M15" s="106" t="s">
         <v>369</v>
@@ -3911,7 +3965,7 @@
         <v>12130.16</v>
       </c>
       <c r="R15" s="143" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="S15" s="128">
         <f t="shared" si="3"/>
@@ -3921,12 +3975,12 @@
         <v>1</v>
       </c>
       <c r="U15" s="130" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="V15" s="130"/>
       <c r="W15" s="130"/>
       <c r="X15" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="Y15" s="128">
         <f t="shared" si="5"/>
@@ -3941,7 +3995,7 @@
         <v>114077</v>
       </c>
       <c r="AB15" s="115" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="16" spans="2:28" ht="51" x14ac:dyDescent="0.2">
@@ -3954,10 +4008,10 @@
         <v>94</v>
       </c>
       <c r="L16" s="106" t="s">
-        <v>7</v>
+        <v>440</v>
       </c>
       <c r="M16" s="106" t="s">
-        <v>369</v>
+        <v>440</v>
       </c>
       <c r="N16" s="123">
         <f t="shared" si="1"/>
@@ -3967,7 +4021,7 @@
         <v>0</v>
       </c>
       <c r="P16" s="133" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q16" s="123">
         <f t="shared" si="2"/>
@@ -4000,12 +4054,12 @@
         <v>0</v>
       </c>
       <c r="AB16" s="115" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="17" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D17" s="16"/>
-      <c r="E17" s="87"/>
+      <c r="E17" s="16"/>
       <c r="J17" s="106" t="s">
         <v>4</v>
       </c>
@@ -4013,7 +4067,7 @@
         <v>94</v>
       </c>
       <c r="L17" s="106" t="s">
-        <v>7</v>
+        <v>439</v>
       </c>
       <c r="M17" s="106" t="s">
         <v>369</v>
@@ -4070,7 +4124,7 @@
         <v>94</v>
       </c>
       <c r="L18" s="106" t="s">
-        <v>7</v>
+        <v>439</v>
       </c>
       <c r="M18" s="106" t="s">
         <v>369</v>
@@ -4088,7 +4142,7 @@
         <v>8583.58</v>
       </c>
       <c r="R18" s="143" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="S18" s="128">
         <f t="shared" si="3"/>
@@ -4098,10 +4152,10 @@
         <v>0.03</v>
       </c>
       <c r="U18" s="130" t="s">
+        <v>411</v>
+      </c>
+      <c r="V18" s="130" t="s">
         <v>412</v>
-      </c>
-      <c r="V18" s="130" t="s">
-        <v>413</v>
       </c>
       <c r="W18" s="130"/>
       <c r="X18" s="130"/>
@@ -4131,7 +4185,7 @@
         <v>94</v>
       </c>
       <c r="L19" s="106" t="s">
-        <v>7</v>
+        <v>439</v>
       </c>
       <c r="M19" s="106" t="s">
         <v>369</v>
@@ -4149,7 +4203,7 @@
         <v>11224.67</v>
       </c>
       <c r="R19" s="143" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="S19" s="128">
         <f t="shared" si="3"/>
@@ -4159,10 +4213,10 @@
         <v>0.03</v>
       </c>
       <c r="U19" s="130" t="s">
+        <v>411</v>
+      </c>
+      <c r="V19" s="130" t="s">
         <v>412</v>
-      </c>
-      <c r="V19" s="130" t="s">
-        <v>413</v>
       </c>
       <c r="W19" s="130"/>
       <c r="X19" s="130"/>
@@ -4210,7 +4264,7 @@
         <v>6910.4</v>
       </c>
       <c r="R20" s="143" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="S20" s="128">
         <f t="shared" si="3"/>
@@ -4220,11 +4274,11 @@
         <v>0.2</v>
       </c>
       <c r="U20" s="130" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="V20" s="130"/>
       <c r="W20" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="X20" s="130"/>
       <c r="Y20" s="128">
@@ -4240,14 +4294,14 @@
         <v>0</v>
       </c>
       <c r="AB20" s="115" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="21" spans="4:28" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="D21" s="16"/>
       <c r="E21" s="87"/>
       <c r="J21" s="106" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K21" s="106" t="s">
         <v>94</v>
@@ -4271,7 +4325,7 @@
         <v>5595.2800000000007</v>
       </c>
       <c r="R21" s="143" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="S21" s="128">
         <f t="shared" si="3"/>
@@ -4281,11 +4335,11 @@
         <v>0.04</v>
       </c>
       <c r="U21" s="130" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="V21" s="130"/>
       <c r="W21" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="X21" s="130"/>
       <c r="Y21" s="128">
@@ -4301,7 +4355,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="115" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="22" spans="4:28" x14ac:dyDescent="0.2">
@@ -4342,12 +4396,12 @@
         <v>0.15</v>
       </c>
       <c r="U22" s="130" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="V22" s="130"/>
       <c r="W22" s="130"/>
       <c r="X22" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="Y22" s="128">
         <f t="shared" si="5"/>
@@ -4362,7 +4416,7 @@
         <v>6620.55</v>
       </c>
       <c r="AB22" s="115" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="23" spans="4:28" x14ac:dyDescent="0.2">
@@ -4403,12 +4457,12 @@
         <v>0.15</v>
       </c>
       <c r="U23" s="130" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="V23" s="130"/>
       <c r="W23" s="130"/>
       <c r="X23" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="Y23" s="128">
         <f t="shared" si="5"/>
@@ -4423,10 +4477,12 @@
         <v>4200.5999999999995</v>
       </c>
       <c r="AB23" s="115" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
-    <row r="24" spans="4:28" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:28" ht="30.6" x14ac:dyDescent="0.2">
+      <c r="D24" s="16"/>
+      <c r="E24" s="87"/>
       <c r="J24" s="106" t="s">
         <v>70</v>
       </c>
@@ -4437,7 +4493,7 @@
         <v>369</v>
       </c>
       <c r="M24" s="106" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N24" s="123">
         <f t="shared" si="1"/>
@@ -4462,12 +4518,12 @@
         <v>0.15</v>
       </c>
       <c r="U24" s="130" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="V24" s="130"/>
       <c r="W24" s="130"/>
       <c r="X24" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="Y24" s="128">
         <f t="shared" si="5"/>
@@ -4482,7 +4538,7 @@
         <v>4430.8499999999995</v>
       </c>
       <c r="AB24" s="115" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="25" spans="4:28" x14ac:dyDescent="0.3">
@@ -4521,12 +4577,12 @@
         <v>0.15</v>
       </c>
       <c r="U25" s="130" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="V25" s="130"/>
       <c r="W25" s="130"/>
       <c r="X25" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="Y25" s="128">
         <f t="shared" si="5"/>
@@ -4541,7 +4597,7 @@
         <v>3084.75</v>
       </c>
       <c r="AB25" s="115" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="26" spans="4:28" x14ac:dyDescent="0.3">
@@ -4580,12 +4636,12 @@
         <v>0.15</v>
       </c>
       <c r="U26" s="130" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="V26" s="130"/>
       <c r="W26" s="130"/>
       <c r="X26" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="Y26" s="128">
         <f t="shared" si="5"/>
@@ -4600,7 +4656,7 @@
         <v>2959.5</v>
       </c>
       <c r="AB26" s="115" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="27" spans="4:28" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -4614,7 +4670,7 @@
         <v>369</v>
       </c>
       <c r="M27" s="106" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="N27" s="123">
         <f t="shared" si="1"/>
@@ -4655,7 +4711,7 @@
         <v>0</v>
       </c>
       <c r="AB27" s="115" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="28" spans="4:28" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -4694,10 +4750,10 @@
         <v>0.15</v>
       </c>
       <c r="U28" s="130" t="s">
+        <v>411</v>
+      </c>
+      <c r="V28" s="130" t="s">
         <v>412</v>
-      </c>
-      <c r="V28" s="130" t="s">
-        <v>413</v>
       </c>
       <c r="W28" s="130"/>
       <c r="X28" s="130"/>
@@ -4714,7 +4770,7 @@
         <v>0</v>
       </c>
       <c r="AB28" s="115" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="29" spans="4:28" x14ac:dyDescent="0.3">
@@ -4753,10 +4809,10 @@
         <v>0.15</v>
       </c>
       <c r="U29" s="130" t="s">
+        <v>411</v>
+      </c>
+      <c r="V29" s="130" t="s">
         <v>412</v>
-      </c>
-      <c r="V29" s="130" t="s">
-        <v>413</v>
       </c>
       <c r="W29" s="130"/>
       <c r="X29" s="130"/>
@@ -4773,7 +4829,7 @@
         <v>0</v>
       </c>
       <c r="AB29" s="115" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="30" spans="4:28" x14ac:dyDescent="0.3">
@@ -4812,11 +4868,11 @@
         <v>0.15</v>
       </c>
       <c r="U30" s="130" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="V30" s="130"/>
       <c r="W30" s="130" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="X30" s="130"/>
       <c r="Y30" s="128">
@@ -4832,7 +4888,7 @@
         <v>0</v>
       </c>
       <c r="AB30" s="115" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="31" spans="4:28" ht="40.799999999999997" x14ac:dyDescent="0.3">
@@ -4856,7 +4912,7 @@
         <v>0</v>
       </c>
       <c r="P31" s="133" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="Q31" s="123">
         <f t="shared" si="2"/>
@@ -4889,7 +4945,7 @@
         <v>0</v>
       </c>
       <c r="AB31" s="115" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="32" spans="4:28" ht="40.799999999999997" x14ac:dyDescent="0.3">
@@ -4913,7 +4969,7 @@
         <v>0</v>
       </c>
       <c r="P32" s="133" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="Q32" s="123">
         <f t="shared" si="2"/>
@@ -4946,7 +5002,7 @@
         <v>0</v>
       </c>
       <c r="AB32" s="115" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="33" spans="10:28" ht="30.6" x14ac:dyDescent="0.3">
@@ -4970,7 +5026,7 @@
         <v>0</v>
       </c>
       <c r="P33" s="133" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q33" s="123">
         <f t="shared" si="2"/>
@@ -5003,7 +5059,7 @@
         <v>0</v>
       </c>
       <c r="AB33" s="115" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="34" spans="10:28" ht="30.6" x14ac:dyDescent="0.3">
@@ -5027,7 +5083,7 @@
         <v>0</v>
       </c>
       <c r="P34" s="134" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q34" s="125">
         <f t="shared" si="2"/>
@@ -5060,13 +5116,13 @@
         <v>0</v>
       </c>
       <c r="AB34" s="117" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="35" spans="10:28" x14ac:dyDescent="0.3">
       <c r="O35" s="122"/>
       <c r="P35" s="135" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="Q35" s="127">
         <f>SUM(Q4:Q34)</f>
@@ -5074,7 +5130,7 @@
       </c>
       <c r="R35" s="113"/>
       <c r="X35" s="142" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="Y35" s="132">
         <f>SUM(Y4:Y34)</f>
@@ -5091,7 +5147,7 @@
     </row>
     <row r="36" spans="10:28" x14ac:dyDescent="0.3">
       <c r="X36" s="142" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="Y36" s="132">
         <f>Y35/1</f>
@@ -5120,11 +5176,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A44" sqref="A44:XFD44"/>
+      <selection pane="bottomRight" activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -8562,7 +8618,7 @@
         <v>53</v>
       </c>
       <c r="I27" s="85" t="s">
-        <v>369</v>
+        <v>53</v>
       </c>
       <c r="J27" s="24" t="s">
         <v>1</v>
@@ -8683,7 +8739,7 @@
         <v>53</v>
       </c>
       <c r="I28" s="85" t="s">
-        <v>369</v>
+        <v>53</v>
       </c>
       <c r="J28" s="24" t="s">
         <v>45</v>
@@ -8801,7 +8857,7 @@
         <v>114</v>
       </c>
       <c r="H29" s="85" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I29" s="85" t="s">
         <v>369</v>
@@ -8922,7 +8978,7 @@
         <v>114</v>
       </c>
       <c r="H30" s="85" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I30" s="85" t="s">
         <v>369</v>
@@ -9043,10 +9099,10 @@
         <v>7</v>
       </c>
       <c r="H31" s="85" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="I31" s="85" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J31" s="24" t="s">
         <v>1</v>
@@ -9164,10 +9220,10 @@
         <v>7</v>
       </c>
       <c r="H32" s="85" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="I32" s="145" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J32" s="24" t="s">
         <v>1</v>
@@ -9285,7 +9341,7 @@
         <v>7</v>
       </c>
       <c r="H33" s="85" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I33" s="85" t="s">
         <v>369</v>
@@ -9406,7 +9462,7 @@
         <v>7</v>
       </c>
       <c r="H34" s="85" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I34" s="85" t="s">
         <v>369</v>
@@ -9527,7 +9583,7 @@
         <v>7</v>
       </c>
       <c r="H35" s="85" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I35" s="85" t="s">
         <v>369</v>
@@ -9748,16 +9804,16 @@
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="C37" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="18" t="s">
         <v>380</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>382</v>
-      </c>
-      <c r="C37" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>381</v>
       </c>
       <c r="E37" s="16" t="s">
         <v>113</v>
@@ -9775,10 +9831,10 @@
         <v>369</v>
       </c>
       <c r="J37" s="24" t="s">
+        <v>382</v>
+      </c>
+      <c r="K37" s="30" t="s">
         <v>383</v>
-      </c>
-      <c r="K37" s="30" t="s">
-        <v>384</v>
       </c>
       <c r="L37" s="57" t="s">
         <v>193</v>
@@ -10984,7 +11040,7 @@
         <v>369</v>
       </c>
       <c r="I47" s="85" t="s">
-        <v>441</v>
+        <v>45</v>
       </c>
       <c r="J47" s="18" t="s">
         <v>1</v>
@@ -12086,8 +12142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A2C2A-A63B-4175-BFD5-FBED9F37A1FC}">
   <dimension ref="A1:AW47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AP19" sqref="AP19:AQ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -18666,7 +18722,7 @@
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E31" sqref="E31:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>